<commit_message>
pulling in latest spreadsheets
</commit_message>
<xml_diff>
--- a/xls/Units.xlsx
+++ b/xls/Units.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Salmon\2018 DBs - Paul Fixes Late Feb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17840" yWindow="0" windowWidth="19360" windowHeight="15520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="room typology" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$S$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$P$243</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1409,12 +1414,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1429,7 +1440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1475,6 +1486,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1748,7 +1770,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1762,459 +1784,459 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="3" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="10.453125" customWidth="1"/>
     <col min="258" max="258" width="29" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="18" customWidth="1"/>
-    <col min="260" max="260" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="262" max="262" width="36" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="10.5" customWidth="1"/>
+    <col min="263" max="263" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="10.453125" customWidth="1"/>
     <col min="514" max="514" width="29" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="18" customWidth="1"/>
-    <col min="516" max="516" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="517" max="517" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="518" max="518" width="36" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="10.5" customWidth="1"/>
+    <col min="519" max="519" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="10.453125" customWidth="1"/>
     <col min="770" max="770" width="29" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="18" customWidth="1"/>
-    <col min="772" max="772" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="773" max="773" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="774" max="774" width="36" bestFit="1" customWidth="1"/>
-    <col min="775" max="775" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="10.5" customWidth="1"/>
+    <col min="775" max="775" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="10.453125" customWidth="1"/>
     <col min="1026" max="1026" width="29" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="18" customWidth="1"/>
-    <col min="1028" max="1028" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1029" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="1030" max="1030" width="36" bestFit="1" customWidth="1"/>
-    <col min="1031" max="1031" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="10.5" customWidth="1"/>
+    <col min="1031" max="1031" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="10.453125" customWidth="1"/>
     <col min="1282" max="1282" width="29" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="18" customWidth="1"/>
-    <col min="1284" max="1284" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="1285" max="1285" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="1286" max="1286" width="36" bestFit="1" customWidth="1"/>
-    <col min="1287" max="1287" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="10.5" customWidth="1"/>
+    <col min="1287" max="1287" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="10.453125" customWidth="1"/>
     <col min="1538" max="1538" width="29" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="18" customWidth="1"/>
-    <col min="1540" max="1540" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="1541" max="1541" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="1542" max="1542" width="36" bestFit="1" customWidth="1"/>
-    <col min="1543" max="1543" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="10.5" customWidth="1"/>
+    <col min="1543" max="1543" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="10.453125" customWidth="1"/>
     <col min="1794" max="1794" width="29" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="18" customWidth="1"/>
-    <col min="1796" max="1796" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="1797" max="1797" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="1798" max="1798" width="36" bestFit="1" customWidth="1"/>
-    <col min="1799" max="1799" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="10.5" customWidth="1"/>
+    <col min="1799" max="1799" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="10.453125" customWidth="1"/>
     <col min="2050" max="2050" width="29" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="18" customWidth="1"/>
-    <col min="2052" max="2052" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="2053" max="2053" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2054" max="2054" width="36" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2055" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="10.5" customWidth="1"/>
+    <col min="2055" max="2055" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="10.453125" customWidth="1"/>
     <col min="2306" max="2306" width="29" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="18" customWidth="1"/>
-    <col min="2308" max="2308" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="2309" max="2309" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2310" max="2310" width="36" bestFit="1" customWidth="1"/>
-    <col min="2311" max="2311" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="10.5" customWidth="1"/>
+    <col min="2311" max="2311" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="10.453125" customWidth="1"/>
     <col min="2562" max="2562" width="29" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="18" customWidth="1"/>
-    <col min="2564" max="2564" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="2565" max="2565" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2566" max="2566" width="36" bestFit="1" customWidth="1"/>
-    <col min="2567" max="2567" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="10.5" customWidth="1"/>
+    <col min="2567" max="2567" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="10.453125" customWidth="1"/>
     <col min="2818" max="2818" width="29" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="18" customWidth="1"/>
-    <col min="2820" max="2820" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="2821" max="2821" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2822" max="2822" width="36" bestFit="1" customWidth="1"/>
-    <col min="2823" max="2823" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="10.5" customWidth="1"/>
+    <col min="2823" max="2823" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="10.453125" customWidth="1"/>
     <col min="3074" max="3074" width="29" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="18" customWidth="1"/>
-    <col min="3076" max="3076" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="3077" max="3077" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="3078" max="3078" width="36" bestFit="1" customWidth="1"/>
-    <col min="3079" max="3079" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="10.5" customWidth="1"/>
+    <col min="3079" max="3079" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="10.453125" customWidth="1"/>
     <col min="3330" max="3330" width="29" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="18" customWidth="1"/>
-    <col min="3332" max="3332" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="3333" max="3333" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="3334" max="3334" width="36" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3335" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="10.5" customWidth="1"/>
+    <col min="3335" max="3335" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="10.453125" customWidth="1"/>
     <col min="3586" max="3586" width="29" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="18" customWidth="1"/>
-    <col min="3588" max="3588" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="3589" max="3589" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="3590" max="3590" width="36" bestFit="1" customWidth="1"/>
-    <col min="3591" max="3591" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="10.5" customWidth="1"/>
+    <col min="3591" max="3591" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="10.453125" customWidth="1"/>
     <col min="3842" max="3842" width="29" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="18" customWidth="1"/>
-    <col min="3844" max="3844" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="3845" max="3845" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="3846" max="3846" width="36" bestFit="1" customWidth="1"/>
-    <col min="3847" max="3847" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="10.5" customWidth="1"/>
+    <col min="3847" max="3847" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="10.453125" customWidth="1"/>
     <col min="4098" max="4098" width="29" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="18" customWidth="1"/>
-    <col min="4100" max="4100" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="4101" max="4101" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="4102" max="4102" width="36" bestFit="1" customWidth="1"/>
-    <col min="4103" max="4103" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="10.5" customWidth="1"/>
+    <col min="4103" max="4103" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="10.453125" customWidth="1"/>
     <col min="4354" max="4354" width="29" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="18" customWidth="1"/>
-    <col min="4356" max="4356" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="4357" max="4357" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="4358" max="4358" width="36" bestFit="1" customWidth="1"/>
-    <col min="4359" max="4359" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="10.5" customWidth="1"/>
+    <col min="4359" max="4359" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="10.453125" customWidth="1"/>
     <col min="4610" max="4610" width="29" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="18" customWidth="1"/>
-    <col min="4612" max="4612" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="4613" max="4613" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="4614" max="4614" width="36" bestFit="1" customWidth="1"/>
-    <col min="4615" max="4615" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="10.5" customWidth="1"/>
+    <col min="4615" max="4615" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="10.453125" customWidth="1"/>
     <col min="4866" max="4866" width="29" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="18" customWidth="1"/>
-    <col min="4868" max="4868" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="4869" max="4869" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="4870" max="4870" width="36" bestFit="1" customWidth="1"/>
-    <col min="4871" max="4871" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="10.5" customWidth="1"/>
+    <col min="4871" max="4871" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="10.453125" customWidth="1"/>
     <col min="5122" max="5122" width="29" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="18" customWidth="1"/>
-    <col min="5124" max="5124" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="5125" max="5125" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="5126" max="5126" width="36" bestFit="1" customWidth="1"/>
-    <col min="5127" max="5127" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="10.5" customWidth="1"/>
+    <col min="5127" max="5127" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="10.453125" customWidth="1"/>
     <col min="5378" max="5378" width="29" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="18" customWidth="1"/>
-    <col min="5380" max="5380" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="5381" max="5381" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="5382" max="5382" width="36" bestFit="1" customWidth="1"/>
-    <col min="5383" max="5383" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="10.5" customWidth="1"/>
+    <col min="5383" max="5383" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="10.453125" customWidth="1"/>
     <col min="5634" max="5634" width="29" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="18" customWidth="1"/>
-    <col min="5636" max="5636" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="5637" max="5637" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="5638" max="5638" width="36" bestFit="1" customWidth="1"/>
-    <col min="5639" max="5639" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="10.5" customWidth="1"/>
+    <col min="5639" max="5639" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="10.453125" customWidth="1"/>
     <col min="5890" max="5890" width="29" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="18" customWidth="1"/>
-    <col min="5892" max="5892" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="5893" max="5893" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="5894" max="5894" width="36" bestFit="1" customWidth="1"/>
-    <col min="5895" max="5895" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="10.5" customWidth="1"/>
+    <col min="5895" max="5895" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="10.453125" customWidth="1"/>
     <col min="6146" max="6146" width="29" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="18" customWidth="1"/>
-    <col min="6148" max="6148" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="6149" max="6149" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="6150" max="6150" width="36" bestFit="1" customWidth="1"/>
-    <col min="6151" max="6151" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="10.5" customWidth="1"/>
+    <col min="6151" max="6151" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="10.453125" customWidth="1"/>
     <col min="6402" max="6402" width="29" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="18" customWidth="1"/>
-    <col min="6404" max="6404" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="6405" max="6405" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="6406" max="6406" width="36" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6407" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="10.5" customWidth="1"/>
+    <col min="6407" max="6407" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="10.453125" customWidth="1"/>
     <col min="6658" max="6658" width="29" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="18" customWidth="1"/>
-    <col min="6660" max="6660" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="6661" max="6661" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="6662" max="6662" width="36" bestFit="1" customWidth="1"/>
-    <col min="6663" max="6663" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="10.5" customWidth="1"/>
+    <col min="6663" max="6663" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="10.453125" customWidth="1"/>
     <col min="6914" max="6914" width="29" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="18" customWidth="1"/>
-    <col min="6916" max="6916" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="6917" max="6917" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="6918" max="6918" width="36" bestFit="1" customWidth="1"/>
-    <col min="6919" max="6919" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="10.5" customWidth="1"/>
+    <col min="6919" max="6919" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="10.453125" customWidth="1"/>
     <col min="7170" max="7170" width="29" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="18" customWidth="1"/>
-    <col min="7172" max="7172" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="7173" max="7173" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="7174" max="7174" width="36" bestFit="1" customWidth="1"/>
-    <col min="7175" max="7175" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="10.5" customWidth="1"/>
+    <col min="7175" max="7175" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="10.453125" customWidth="1"/>
     <col min="7426" max="7426" width="29" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="18" customWidth="1"/>
-    <col min="7428" max="7428" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="7429" max="7429" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="7430" max="7430" width="36" bestFit="1" customWidth="1"/>
-    <col min="7431" max="7431" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="10.5" customWidth="1"/>
+    <col min="7431" max="7431" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="10.453125" customWidth="1"/>
     <col min="7682" max="7682" width="29" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="18" customWidth="1"/>
-    <col min="7684" max="7684" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="7685" max="7685" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="7686" max="7686" width="36" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7687" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="10.5" customWidth="1"/>
+    <col min="7687" max="7687" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="10.453125" customWidth="1"/>
     <col min="7938" max="7938" width="29" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="18" customWidth="1"/>
-    <col min="7940" max="7940" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="7941" max="7941" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="7942" max="7942" width="36" bestFit="1" customWidth="1"/>
-    <col min="7943" max="7943" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="10.5" customWidth="1"/>
+    <col min="7943" max="7943" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="10.453125" customWidth="1"/>
     <col min="8194" max="8194" width="29" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="18" customWidth="1"/>
-    <col min="8196" max="8196" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="8197" max="8197" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="8198" max="8198" width="36" bestFit="1" customWidth="1"/>
-    <col min="8199" max="8199" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="10.5" customWidth="1"/>
+    <col min="8199" max="8199" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="10.453125" customWidth="1"/>
     <col min="8450" max="8450" width="29" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="18" customWidth="1"/>
-    <col min="8452" max="8452" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="8453" max="8453" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="8454" max="8454" width="36" bestFit="1" customWidth="1"/>
-    <col min="8455" max="8455" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="10.5" customWidth="1"/>
+    <col min="8455" max="8455" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="10.453125" customWidth="1"/>
     <col min="8706" max="8706" width="29" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="18" customWidth="1"/>
-    <col min="8708" max="8708" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="8709" max="8709" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="8710" max="8710" width="36" bestFit="1" customWidth="1"/>
-    <col min="8711" max="8711" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="10.5" customWidth="1"/>
+    <col min="8711" max="8711" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="10.453125" customWidth="1"/>
     <col min="8962" max="8962" width="29" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="18" customWidth="1"/>
-    <col min="8964" max="8964" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="8965" max="8965" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="8966" max="8966" width="36" bestFit="1" customWidth="1"/>
-    <col min="8967" max="8967" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="10.5" customWidth="1"/>
+    <col min="8967" max="8967" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="10.453125" customWidth="1"/>
     <col min="9218" max="9218" width="29" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="18" customWidth="1"/>
-    <col min="9220" max="9220" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="9221" max="9221" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="9222" max="9222" width="36" bestFit="1" customWidth="1"/>
-    <col min="9223" max="9223" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="10.5" customWidth="1"/>
+    <col min="9223" max="9223" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="10.453125" customWidth="1"/>
     <col min="9474" max="9474" width="29" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="18" customWidth="1"/>
-    <col min="9476" max="9476" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="9477" max="9477" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="9478" max="9478" width="36" bestFit="1" customWidth="1"/>
-    <col min="9479" max="9479" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="10.5" customWidth="1"/>
+    <col min="9479" max="9479" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="10.453125" customWidth="1"/>
     <col min="9730" max="9730" width="29" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="18" customWidth="1"/>
-    <col min="9732" max="9732" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="9733" max="9733" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="9734" max="9734" width="36" bestFit="1" customWidth="1"/>
-    <col min="9735" max="9735" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="10.5" customWidth="1"/>
+    <col min="9735" max="9735" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="10.453125" customWidth="1"/>
     <col min="9986" max="9986" width="29" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="18" customWidth="1"/>
-    <col min="9988" max="9988" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="9989" max="9989" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="9990" max="9990" width="36" bestFit="1" customWidth="1"/>
-    <col min="9991" max="9991" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="10.5" customWidth="1"/>
+    <col min="9991" max="9991" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="10.453125" customWidth="1"/>
     <col min="10242" max="10242" width="29" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="18" customWidth="1"/>
-    <col min="10244" max="10244" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="10245" max="10245" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="10246" max="10246" width="36" bestFit="1" customWidth="1"/>
-    <col min="10247" max="10247" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="10.5" customWidth="1"/>
+    <col min="10247" max="10247" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="10.453125" customWidth="1"/>
     <col min="10498" max="10498" width="29" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="18" customWidth="1"/>
-    <col min="10500" max="10500" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="10501" max="10501" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="10502" max="10502" width="36" bestFit="1" customWidth="1"/>
-    <col min="10503" max="10503" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="10.5" customWidth="1"/>
+    <col min="10503" max="10503" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="10.453125" customWidth="1"/>
     <col min="10754" max="10754" width="29" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="18" customWidth="1"/>
-    <col min="10756" max="10756" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="10757" max="10757" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="10758" max="10758" width="36" bestFit="1" customWidth="1"/>
-    <col min="10759" max="10759" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="10.5" customWidth="1"/>
+    <col min="10759" max="10759" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="10.453125" customWidth="1"/>
     <col min="11010" max="11010" width="29" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="18" customWidth="1"/>
-    <col min="11012" max="11012" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="11013" max="11013" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="11014" max="11014" width="36" bestFit="1" customWidth="1"/>
-    <col min="11015" max="11015" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="10.5" customWidth="1"/>
+    <col min="11015" max="11015" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="10.453125" customWidth="1"/>
     <col min="11266" max="11266" width="29" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="18" customWidth="1"/>
-    <col min="11268" max="11268" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="11269" max="11269" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="11270" max="11270" width="36" bestFit="1" customWidth="1"/>
-    <col min="11271" max="11271" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="10.5" customWidth="1"/>
+    <col min="11271" max="11271" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="10.453125" customWidth="1"/>
     <col min="11522" max="11522" width="29" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="18" customWidth="1"/>
-    <col min="11524" max="11524" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="11525" max="11525" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="11526" max="11526" width="36" bestFit="1" customWidth="1"/>
-    <col min="11527" max="11527" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="10.5" customWidth="1"/>
+    <col min="11527" max="11527" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="10.453125" customWidth="1"/>
     <col min="11778" max="11778" width="29" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="18" customWidth="1"/>
-    <col min="11780" max="11780" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="11781" max="11781" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="11782" max="11782" width="36" bestFit="1" customWidth="1"/>
-    <col min="11783" max="11783" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="10.5" customWidth="1"/>
+    <col min="11783" max="11783" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="10.453125" customWidth="1"/>
     <col min="12034" max="12034" width="29" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="18" customWidth="1"/>
-    <col min="12036" max="12036" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="12037" max="12037" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="12038" max="12038" width="36" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12039" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="10.5" customWidth="1"/>
+    <col min="12039" max="12039" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="10.453125" customWidth="1"/>
     <col min="12290" max="12290" width="29" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="18" customWidth="1"/>
-    <col min="12292" max="12292" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="12293" max="12293" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="12294" max="12294" width="36" bestFit="1" customWidth="1"/>
-    <col min="12295" max="12295" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="10.5" customWidth="1"/>
+    <col min="12295" max="12295" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="10.453125" customWidth="1"/>
     <col min="12546" max="12546" width="29" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="18" customWidth="1"/>
-    <col min="12548" max="12548" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="12549" max="12549" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="12550" max="12550" width="36" bestFit="1" customWidth="1"/>
-    <col min="12551" max="12551" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="10.5" customWidth="1"/>
+    <col min="12551" max="12551" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="10.453125" customWidth="1"/>
     <col min="12802" max="12802" width="29" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="18" customWidth="1"/>
-    <col min="12804" max="12804" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="12805" max="12805" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="12806" max="12806" width="36" bestFit="1" customWidth="1"/>
-    <col min="12807" max="12807" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="10.5" customWidth="1"/>
+    <col min="12807" max="12807" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="10.453125" customWidth="1"/>
     <col min="13058" max="13058" width="29" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="18" customWidth="1"/>
-    <col min="13060" max="13060" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="13061" max="13061" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="13062" max="13062" width="36" bestFit="1" customWidth="1"/>
-    <col min="13063" max="13063" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="10.5" customWidth="1"/>
+    <col min="13063" max="13063" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="10.453125" customWidth="1"/>
     <col min="13314" max="13314" width="29" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="18" customWidth="1"/>
-    <col min="13316" max="13316" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13317" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="13318" max="13318" width="36" bestFit="1" customWidth="1"/>
-    <col min="13319" max="13319" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="10.5" customWidth="1"/>
+    <col min="13319" max="13319" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="10.453125" customWidth="1"/>
     <col min="13570" max="13570" width="29" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="18" customWidth="1"/>
-    <col min="13572" max="13572" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="13573" max="13573" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="13574" max="13574" width="36" bestFit="1" customWidth="1"/>
-    <col min="13575" max="13575" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="10.5" customWidth="1"/>
+    <col min="13575" max="13575" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="10.453125" customWidth="1"/>
     <col min="13826" max="13826" width="29" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="18" customWidth="1"/>
-    <col min="13828" max="13828" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="13829" max="13829" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="13830" max="13830" width="36" bestFit="1" customWidth="1"/>
-    <col min="13831" max="13831" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="10.5" customWidth="1"/>
+    <col min="13831" max="13831" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="10.453125" customWidth="1"/>
     <col min="14082" max="14082" width="29" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="18" customWidth="1"/>
-    <col min="14084" max="14084" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="14085" max="14085" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="14086" max="14086" width="36" bestFit="1" customWidth="1"/>
-    <col min="14087" max="14087" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="10.5" customWidth="1"/>
+    <col min="14087" max="14087" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="10.453125" customWidth="1"/>
     <col min="14338" max="14338" width="29" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="18" customWidth="1"/>
-    <col min="14340" max="14340" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="14341" max="14341" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="14342" max="14342" width="36" bestFit="1" customWidth="1"/>
-    <col min="14343" max="14343" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="10.5" customWidth="1"/>
+    <col min="14343" max="14343" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="10.453125" customWidth="1"/>
     <col min="14594" max="14594" width="29" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="18" customWidth="1"/>
-    <col min="14596" max="14596" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="14597" max="14597" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="14598" max="14598" width="36" bestFit="1" customWidth="1"/>
-    <col min="14599" max="14599" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="10.5" customWidth="1"/>
+    <col min="14599" max="14599" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="10.453125" customWidth="1"/>
     <col min="14850" max="14850" width="29" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="18" customWidth="1"/>
-    <col min="14852" max="14852" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="14853" max="14853" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="14854" max="14854" width="36" bestFit="1" customWidth="1"/>
-    <col min="14855" max="14855" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="10.5" customWidth="1"/>
+    <col min="14855" max="14855" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="10.453125" customWidth="1"/>
     <col min="15106" max="15106" width="29" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="18" customWidth="1"/>
-    <col min="15108" max="15108" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="15109" max="15109" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="15110" max="15110" width="36" bestFit="1" customWidth="1"/>
-    <col min="15111" max="15111" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="10.5" customWidth="1"/>
+    <col min="15111" max="15111" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="10.453125" customWidth="1"/>
     <col min="15362" max="15362" width="29" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="18" customWidth="1"/>
-    <col min="15364" max="15364" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="15365" max="15365" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="15366" max="15366" width="36" bestFit="1" customWidth="1"/>
-    <col min="15367" max="15367" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="10.5" customWidth="1"/>
+    <col min="15367" max="15367" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="10.453125" customWidth="1"/>
     <col min="15618" max="15618" width="29" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="18" customWidth="1"/>
-    <col min="15620" max="15620" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="15621" max="15621" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="15622" max="15622" width="36" bestFit="1" customWidth="1"/>
-    <col min="15623" max="15623" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="10.5" customWidth="1"/>
+    <col min="15623" max="15623" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="10.453125" customWidth="1"/>
     <col min="15874" max="15874" width="29" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="18" customWidth="1"/>
-    <col min="15876" max="15876" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="15877" max="15877" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="15878" max="15878" width="36" bestFit="1" customWidth="1"/>
-    <col min="15879" max="15879" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="10.5" customWidth="1"/>
+    <col min="15879" max="15879" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="10.453125" customWidth="1"/>
     <col min="16130" max="16130" width="29" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="18" customWidth="1"/>
-    <col min="16132" max="16132" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="59.453125" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="16134" max="16134" width="36" bestFit="1" customWidth="1"/>
-    <col min="16135" max="16135" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="12">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2242,7 +2264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2256,7 +2278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2270,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2284,7 +2306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2298,7 +2320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2312,7 +2334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2326,7 +2348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2340,7 +2362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2354,7 +2376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2368,7 +2390,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2382,7 +2404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2396,7 +2418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2410,7 +2432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2438,913 +2460,913 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K171" sqref="K171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="9" customWidth="1"/>
-    <col min="13" max="14" width="8.83203125" style="3"/>
-    <col min="15" max="15" width="15.5" style="11" customWidth="1"/>
-    <col min="16" max="16" width="36.33203125" style="10" customWidth="1"/>
-    <col min="257" max="257" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.36328125" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="23.1796875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="9" customWidth="1"/>
+    <col min="13" max="14" width="8.81640625" style="3"/>
+    <col min="15" max="15" width="15.453125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="36.36328125" style="10" customWidth="1"/>
+    <col min="257" max="257" width="8.1796875" customWidth="1"/>
     <col min="258" max="258" width="13" customWidth="1"/>
-    <col min="259" max="259" width="11.5" customWidth="1"/>
-    <col min="260" max="260" width="9.5" customWidth="1"/>
-    <col min="261" max="261" width="7.33203125" customWidth="1"/>
-    <col min="262" max="262" width="6.5" customWidth="1"/>
-    <col min="263" max="263" width="10.5" customWidth="1"/>
-    <col min="264" max="264" width="20.33203125" customWidth="1"/>
-    <col min="265" max="265" width="14.83203125" customWidth="1"/>
-    <col min="266" max="266" width="12.1640625" customWidth="1"/>
-    <col min="267" max="267" width="18.6640625" customWidth="1"/>
-    <col min="268" max="268" width="8.83203125" customWidth="1"/>
-    <col min="271" max="271" width="12.83203125" customWidth="1"/>
-    <col min="272" max="272" width="36.33203125" customWidth="1"/>
-    <col min="513" max="513" width="8.1640625" customWidth="1"/>
+    <col min="259" max="259" width="11.453125" customWidth="1"/>
+    <col min="260" max="260" width="9.453125" customWidth="1"/>
+    <col min="261" max="261" width="7.36328125" customWidth="1"/>
+    <col min="262" max="262" width="6.453125" customWidth="1"/>
+    <col min="263" max="263" width="10.453125" customWidth="1"/>
+    <col min="264" max="264" width="20.36328125" customWidth="1"/>
+    <col min="265" max="265" width="14.81640625" customWidth="1"/>
+    <col min="266" max="266" width="12.1796875" customWidth="1"/>
+    <col min="267" max="267" width="18.6328125" customWidth="1"/>
+    <col min="268" max="268" width="8.81640625" customWidth="1"/>
+    <col min="271" max="271" width="12.81640625" customWidth="1"/>
+    <col min="272" max="272" width="36.36328125" customWidth="1"/>
+    <col min="513" max="513" width="8.1796875" customWidth="1"/>
     <col min="514" max="514" width="13" customWidth="1"/>
-    <col min="515" max="515" width="11.5" customWidth="1"/>
-    <col min="516" max="516" width="9.5" customWidth="1"/>
-    <col min="517" max="517" width="7.33203125" customWidth="1"/>
-    <col min="518" max="518" width="6.5" customWidth="1"/>
-    <col min="519" max="519" width="10.5" customWidth="1"/>
-    <col min="520" max="520" width="20.33203125" customWidth="1"/>
-    <col min="521" max="521" width="14.83203125" customWidth="1"/>
-    <col min="522" max="522" width="12.1640625" customWidth="1"/>
-    <col min="523" max="523" width="18.6640625" customWidth="1"/>
-    <col min="524" max="524" width="8.83203125" customWidth="1"/>
-    <col min="527" max="527" width="12.83203125" customWidth="1"/>
-    <col min="528" max="528" width="36.33203125" customWidth="1"/>
-    <col min="769" max="769" width="8.1640625" customWidth="1"/>
+    <col min="515" max="515" width="11.453125" customWidth="1"/>
+    <col min="516" max="516" width="9.453125" customWidth="1"/>
+    <col min="517" max="517" width="7.36328125" customWidth="1"/>
+    <col min="518" max="518" width="6.453125" customWidth="1"/>
+    <col min="519" max="519" width="10.453125" customWidth="1"/>
+    <col min="520" max="520" width="20.36328125" customWidth="1"/>
+    <col min="521" max="521" width="14.81640625" customWidth="1"/>
+    <col min="522" max="522" width="12.1796875" customWidth="1"/>
+    <col min="523" max="523" width="18.6328125" customWidth="1"/>
+    <col min="524" max="524" width="8.81640625" customWidth="1"/>
+    <col min="527" max="527" width="12.81640625" customWidth="1"/>
+    <col min="528" max="528" width="36.36328125" customWidth="1"/>
+    <col min="769" max="769" width="8.1796875" customWidth="1"/>
     <col min="770" max="770" width="13" customWidth="1"/>
-    <col min="771" max="771" width="11.5" customWidth="1"/>
-    <col min="772" max="772" width="9.5" customWidth="1"/>
-    <col min="773" max="773" width="7.33203125" customWidth="1"/>
-    <col min="774" max="774" width="6.5" customWidth="1"/>
-    <col min="775" max="775" width="10.5" customWidth="1"/>
-    <col min="776" max="776" width="20.33203125" customWidth="1"/>
-    <col min="777" max="777" width="14.83203125" customWidth="1"/>
-    <col min="778" max="778" width="12.1640625" customWidth="1"/>
-    <col min="779" max="779" width="18.6640625" customWidth="1"/>
-    <col min="780" max="780" width="8.83203125" customWidth="1"/>
-    <col min="783" max="783" width="12.83203125" customWidth="1"/>
-    <col min="784" max="784" width="36.33203125" customWidth="1"/>
-    <col min="1025" max="1025" width="8.1640625" customWidth="1"/>
+    <col min="771" max="771" width="11.453125" customWidth="1"/>
+    <col min="772" max="772" width="9.453125" customWidth="1"/>
+    <col min="773" max="773" width="7.36328125" customWidth="1"/>
+    <col min="774" max="774" width="6.453125" customWidth="1"/>
+    <col min="775" max="775" width="10.453125" customWidth="1"/>
+    <col min="776" max="776" width="20.36328125" customWidth="1"/>
+    <col min="777" max="777" width="14.81640625" customWidth="1"/>
+    <col min="778" max="778" width="12.1796875" customWidth="1"/>
+    <col min="779" max="779" width="18.6328125" customWidth="1"/>
+    <col min="780" max="780" width="8.81640625" customWidth="1"/>
+    <col min="783" max="783" width="12.81640625" customWidth="1"/>
+    <col min="784" max="784" width="36.36328125" customWidth="1"/>
+    <col min="1025" max="1025" width="8.1796875" customWidth="1"/>
     <col min="1026" max="1026" width="13" customWidth="1"/>
-    <col min="1027" max="1027" width="11.5" customWidth="1"/>
-    <col min="1028" max="1028" width="9.5" customWidth="1"/>
-    <col min="1029" max="1029" width="7.33203125" customWidth="1"/>
-    <col min="1030" max="1030" width="6.5" customWidth="1"/>
-    <col min="1031" max="1031" width="10.5" customWidth="1"/>
-    <col min="1032" max="1032" width="20.33203125" customWidth="1"/>
-    <col min="1033" max="1033" width="14.83203125" customWidth="1"/>
-    <col min="1034" max="1034" width="12.1640625" customWidth="1"/>
-    <col min="1035" max="1035" width="18.6640625" customWidth="1"/>
-    <col min="1036" max="1036" width="8.83203125" customWidth="1"/>
-    <col min="1039" max="1039" width="12.83203125" customWidth="1"/>
-    <col min="1040" max="1040" width="36.33203125" customWidth="1"/>
-    <col min="1281" max="1281" width="8.1640625" customWidth="1"/>
+    <col min="1027" max="1027" width="11.453125" customWidth="1"/>
+    <col min="1028" max="1028" width="9.453125" customWidth="1"/>
+    <col min="1029" max="1029" width="7.36328125" customWidth="1"/>
+    <col min="1030" max="1030" width="6.453125" customWidth="1"/>
+    <col min="1031" max="1031" width="10.453125" customWidth="1"/>
+    <col min="1032" max="1032" width="20.36328125" customWidth="1"/>
+    <col min="1033" max="1033" width="14.81640625" customWidth="1"/>
+    <col min="1034" max="1034" width="12.1796875" customWidth="1"/>
+    <col min="1035" max="1035" width="18.6328125" customWidth="1"/>
+    <col min="1036" max="1036" width="8.81640625" customWidth="1"/>
+    <col min="1039" max="1039" width="12.81640625" customWidth="1"/>
+    <col min="1040" max="1040" width="36.36328125" customWidth="1"/>
+    <col min="1281" max="1281" width="8.1796875" customWidth="1"/>
     <col min="1282" max="1282" width="13" customWidth="1"/>
-    <col min="1283" max="1283" width="11.5" customWidth="1"/>
-    <col min="1284" max="1284" width="9.5" customWidth="1"/>
-    <col min="1285" max="1285" width="7.33203125" customWidth="1"/>
-    <col min="1286" max="1286" width="6.5" customWidth="1"/>
-    <col min="1287" max="1287" width="10.5" customWidth="1"/>
-    <col min="1288" max="1288" width="20.33203125" customWidth="1"/>
-    <col min="1289" max="1289" width="14.83203125" customWidth="1"/>
-    <col min="1290" max="1290" width="12.1640625" customWidth="1"/>
-    <col min="1291" max="1291" width="18.6640625" customWidth="1"/>
-    <col min="1292" max="1292" width="8.83203125" customWidth="1"/>
-    <col min="1295" max="1295" width="12.83203125" customWidth="1"/>
-    <col min="1296" max="1296" width="36.33203125" customWidth="1"/>
-    <col min="1537" max="1537" width="8.1640625" customWidth="1"/>
+    <col min="1283" max="1283" width="11.453125" customWidth="1"/>
+    <col min="1284" max="1284" width="9.453125" customWidth="1"/>
+    <col min="1285" max="1285" width="7.36328125" customWidth="1"/>
+    <col min="1286" max="1286" width="6.453125" customWidth="1"/>
+    <col min="1287" max="1287" width="10.453125" customWidth="1"/>
+    <col min="1288" max="1288" width="20.36328125" customWidth="1"/>
+    <col min="1289" max="1289" width="14.81640625" customWidth="1"/>
+    <col min="1290" max="1290" width="12.1796875" customWidth="1"/>
+    <col min="1291" max="1291" width="18.6328125" customWidth="1"/>
+    <col min="1292" max="1292" width="8.81640625" customWidth="1"/>
+    <col min="1295" max="1295" width="12.81640625" customWidth="1"/>
+    <col min="1296" max="1296" width="36.36328125" customWidth="1"/>
+    <col min="1537" max="1537" width="8.1796875" customWidth="1"/>
     <col min="1538" max="1538" width="13" customWidth="1"/>
-    <col min="1539" max="1539" width="11.5" customWidth="1"/>
-    <col min="1540" max="1540" width="9.5" customWidth="1"/>
-    <col min="1541" max="1541" width="7.33203125" customWidth="1"/>
-    <col min="1542" max="1542" width="6.5" customWidth="1"/>
-    <col min="1543" max="1543" width="10.5" customWidth="1"/>
-    <col min="1544" max="1544" width="20.33203125" customWidth="1"/>
-    <col min="1545" max="1545" width="14.83203125" customWidth="1"/>
-    <col min="1546" max="1546" width="12.1640625" customWidth="1"/>
-    <col min="1547" max="1547" width="18.6640625" customWidth="1"/>
-    <col min="1548" max="1548" width="8.83203125" customWidth="1"/>
-    <col min="1551" max="1551" width="12.83203125" customWidth="1"/>
-    <col min="1552" max="1552" width="36.33203125" customWidth="1"/>
-    <col min="1793" max="1793" width="8.1640625" customWidth="1"/>
+    <col min="1539" max="1539" width="11.453125" customWidth="1"/>
+    <col min="1540" max="1540" width="9.453125" customWidth="1"/>
+    <col min="1541" max="1541" width="7.36328125" customWidth="1"/>
+    <col min="1542" max="1542" width="6.453125" customWidth="1"/>
+    <col min="1543" max="1543" width="10.453125" customWidth="1"/>
+    <col min="1544" max="1544" width="20.36328125" customWidth="1"/>
+    <col min="1545" max="1545" width="14.81640625" customWidth="1"/>
+    <col min="1546" max="1546" width="12.1796875" customWidth="1"/>
+    <col min="1547" max="1547" width="18.6328125" customWidth="1"/>
+    <col min="1548" max="1548" width="8.81640625" customWidth="1"/>
+    <col min="1551" max="1551" width="12.81640625" customWidth="1"/>
+    <col min="1552" max="1552" width="36.36328125" customWidth="1"/>
+    <col min="1793" max="1793" width="8.1796875" customWidth="1"/>
     <col min="1794" max="1794" width="13" customWidth="1"/>
-    <col min="1795" max="1795" width="11.5" customWidth="1"/>
-    <col min="1796" max="1796" width="9.5" customWidth="1"/>
-    <col min="1797" max="1797" width="7.33203125" customWidth="1"/>
-    <col min="1798" max="1798" width="6.5" customWidth="1"/>
-    <col min="1799" max="1799" width="10.5" customWidth="1"/>
-    <col min="1800" max="1800" width="20.33203125" customWidth="1"/>
-    <col min="1801" max="1801" width="14.83203125" customWidth="1"/>
-    <col min="1802" max="1802" width="12.1640625" customWidth="1"/>
-    <col min="1803" max="1803" width="18.6640625" customWidth="1"/>
-    <col min="1804" max="1804" width="8.83203125" customWidth="1"/>
-    <col min="1807" max="1807" width="12.83203125" customWidth="1"/>
-    <col min="1808" max="1808" width="36.33203125" customWidth="1"/>
-    <col min="2049" max="2049" width="8.1640625" customWidth="1"/>
+    <col min="1795" max="1795" width="11.453125" customWidth="1"/>
+    <col min="1796" max="1796" width="9.453125" customWidth="1"/>
+    <col min="1797" max="1797" width="7.36328125" customWidth="1"/>
+    <col min="1798" max="1798" width="6.453125" customWidth="1"/>
+    <col min="1799" max="1799" width="10.453125" customWidth="1"/>
+    <col min="1800" max="1800" width="20.36328125" customWidth="1"/>
+    <col min="1801" max="1801" width="14.81640625" customWidth="1"/>
+    <col min="1802" max="1802" width="12.1796875" customWidth="1"/>
+    <col min="1803" max="1803" width="18.6328125" customWidth="1"/>
+    <col min="1804" max="1804" width="8.81640625" customWidth="1"/>
+    <col min="1807" max="1807" width="12.81640625" customWidth="1"/>
+    <col min="1808" max="1808" width="36.36328125" customWidth="1"/>
+    <col min="2049" max="2049" width="8.1796875" customWidth="1"/>
     <col min="2050" max="2050" width="13" customWidth="1"/>
-    <col min="2051" max="2051" width="11.5" customWidth="1"/>
-    <col min="2052" max="2052" width="9.5" customWidth="1"/>
-    <col min="2053" max="2053" width="7.33203125" customWidth="1"/>
-    <col min="2054" max="2054" width="6.5" customWidth="1"/>
-    <col min="2055" max="2055" width="10.5" customWidth="1"/>
-    <col min="2056" max="2056" width="20.33203125" customWidth="1"/>
-    <col min="2057" max="2057" width="14.83203125" customWidth="1"/>
-    <col min="2058" max="2058" width="12.1640625" customWidth="1"/>
-    <col min="2059" max="2059" width="18.6640625" customWidth="1"/>
-    <col min="2060" max="2060" width="8.83203125" customWidth="1"/>
-    <col min="2063" max="2063" width="12.83203125" customWidth="1"/>
-    <col min="2064" max="2064" width="36.33203125" customWidth="1"/>
-    <col min="2305" max="2305" width="8.1640625" customWidth="1"/>
+    <col min="2051" max="2051" width="11.453125" customWidth="1"/>
+    <col min="2052" max="2052" width="9.453125" customWidth="1"/>
+    <col min="2053" max="2053" width="7.36328125" customWidth="1"/>
+    <col min="2054" max="2054" width="6.453125" customWidth="1"/>
+    <col min="2055" max="2055" width="10.453125" customWidth="1"/>
+    <col min="2056" max="2056" width="20.36328125" customWidth="1"/>
+    <col min="2057" max="2057" width="14.81640625" customWidth="1"/>
+    <col min="2058" max="2058" width="12.1796875" customWidth="1"/>
+    <col min="2059" max="2059" width="18.6328125" customWidth="1"/>
+    <col min="2060" max="2060" width="8.81640625" customWidth="1"/>
+    <col min="2063" max="2063" width="12.81640625" customWidth="1"/>
+    <col min="2064" max="2064" width="36.36328125" customWidth="1"/>
+    <col min="2305" max="2305" width="8.1796875" customWidth="1"/>
     <col min="2306" max="2306" width="13" customWidth="1"/>
-    <col min="2307" max="2307" width="11.5" customWidth="1"/>
-    <col min="2308" max="2308" width="9.5" customWidth="1"/>
-    <col min="2309" max="2309" width="7.33203125" customWidth="1"/>
-    <col min="2310" max="2310" width="6.5" customWidth="1"/>
-    <col min="2311" max="2311" width="10.5" customWidth="1"/>
-    <col min="2312" max="2312" width="20.33203125" customWidth="1"/>
-    <col min="2313" max="2313" width="14.83203125" customWidth="1"/>
-    <col min="2314" max="2314" width="12.1640625" customWidth="1"/>
-    <col min="2315" max="2315" width="18.6640625" customWidth="1"/>
-    <col min="2316" max="2316" width="8.83203125" customWidth="1"/>
-    <col min="2319" max="2319" width="12.83203125" customWidth="1"/>
-    <col min="2320" max="2320" width="36.33203125" customWidth="1"/>
-    <col min="2561" max="2561" width="8.1640625" customWidth="1"/>
+    <col min="2307" max="2307" width="11.453125" customWidth="1"/>
+    <col min="2308" max="2308" width="9.453125" customWidth="1"/>
+    <col min="2309" max="2309" width="7.36328125" customWidth="1"/>
+    <col min="2310" max="2310" width="6.453125" customWidth="1"/>
+    <col min="2311" max="2311" width="10.453125" customWidth="1"/>
+    <col min="2312" max="2312" width="20.36328125" customWidth="1"/>
+    <col min="2313" max="2313" width="14.81640625" customWidth="1"/>
+    <col min="2314" max="2314" width="12.1796875" customWidth="1"/>
+    <col min="2315" max="2315" width="18.6328125" customWidth="1"/>
+    <col min="2316" max="2316" width="8.81640625" customWidth="1"/>
+    <col min="2319" max="2319" width="12.81640625" customWidth="1"/>
+    <col min="2320" max="2320" width="36.36328125" customWidth="1"/>
+    <col min="2561" max="2561" width="8.1796875" customWidth="1"/>
     <col min="2562" max="2562" width="13" customWidth="1"/>
-    <col min="2563" max="2563" width="11.5" customWidth="1"/>
-    <col min="2564" max="2564" width="9.5" customWidth="1"/>
-    <col min="2565" max="2565" width="7.33203125" customWidth="1"/>
-    <col min="2566" max="2566" width="6.5" customWidth="1"/>
-    <col min="2567" max="2567" width="10.5" customWidth="1"/>
-    <col min="2568" max="2568" width="20.33203125" customWidth="1"/>
-    <col min="2569" max="2569" width="14.83203125" customWidth="1"/>
-    <col min="2570" max="2570" width="12.1640625" customWidth="1"/>
-    <col min="2571" max="2571" width="18.6640625" customWidth="1"/>
-    <col min="2572" max="2572" width="8.83203125" customWidth="1"/>
-    <col min="2575" max="2575" width="12.83203125" customWidth="1"/>
-    <col min="2576" max="2576" width="36.33203125" customWidth="1"/>
-    <col min="2817" max="2817" width="8.1640625" customWidth="1"/>
+    <col min="2563" max="2563" width="11.453125" customWidth="1"/>
+    <col min="2564" max="2564" width="9.453125" customWidth="1"/>
+    <col min="2565" max="2565" width="7.36328125" customWidth="1"/>
+    <col min="2566" max="2566" width="6.453125" customWidth="1"/>
+    <col min="2567" max="2567" width="10.453125" customWidth="1"/>
+    <col min="2568" max="2568" width="20.36328125" customWidth="1"/>
+    <col min="2569" max="2569" width="14.81640625" customWidth="1"/>
+    <col min="2570" max="2570" width="12.1796875" customWidth="1"/>
+    <col min="2571" max="2571" width="18.6328125" customWidth="1"/>
+    <col min="2572" max="2572" width="8.81640625" customWidth="1"/>
+    <col min="2575" max="2575" width="12.81640625" customWidth="1"/>
+    <col min="2576" max="2576" width="36.36328125" customWidth="1"/>
+    <col min="2817" max="2817" width="8.1796875" customWidth="1"/>
     <col min="2818" max="2818" width="13" customWidth="1"/>
-    <col min="2819" max="2819" width="11.5" customWidth="1"/>
-    <col min="2820" max="2820" width="9.5" customWidth="1"/>
-    <col min="2821" max="2821" width="7.33203125" customWidth="1"/>
-    <col min="2822" max="2822" width="6.5" customWidth="1"/>
-    <col min="2823" max="2823" width="10.5" customWidth="1"/>
-    <col min="2824" max="2824" width="20.33203125" customWidth="1"/>
-    <col min="2825" max="2825" width="14.83203125" customWidth="1"/>
-    <col min="2826" max="2826" width="12.1640625" customWidth="1"/>
-    <col min="2827" max="2827" width="18.6640625" customWidth="1"/>
-    <col min="2828" max="2828" width="8.83203125" customWidth="1"/>
-    <col min="2831" max="2831" width="12.83203125" customWidth="1"/>
-    <col min="2832" max="2832" width="36.33203125" customWidth="1"/>
-    <col min="3073" max="3073" width="8.1640625" customWidth="1"/>
+    <col min="2819" max="2819" width="11.453125" customWidth="1"/>
+    <col min="2820" max="2820" width="9.453125" customWidth="1"/>
+    <col min="2821" max="2821" width="7.36328125" customWidth="1"/>
+    <col min="2822" max="2822" width="6.453125" customWidth="1"/>
+    <col min="2823" max="2823" width="10.453125" customWidth="1"/>
+    <col min="2824" max="2824" width="20.36328125" customWidth="1"/>
+    <col min="2825" max="2825" width="14.81640625" customWidth="1"/>
+    <col min="2826" max="2826" width="12.1796875" customWidth="1"/>
+    <col min="2827" max="2827" width="18.6328125" customWidth="1"/>
+    <col min="2828" max="2828" width="8.81640625" customWidth="1"/>
+    <col min="2831" max="2831" width="12.81640625" customWidth="1"/>
+    <col min="2832" max="2832" width="36.36328125" customWidth="1"/>
+    <col min="3073" max="3073" width="8.1796875" customWidth="1"/>
     <col min="3074" max="3074" width="13" customWidth="1"/>
-    <col min="3075" max="3075" width="11.5" customWidth="1"/>
-    <col min="3076" max="3076" width="9.5" customWidth="1"/>
-    <col min="3077" max="3077" width="7.33203125" customWidth="1"/>
-    <col min="3078" max="3078" width="6.5" customWidth="1"/>
-    <col min="3079" max="3079" width="10.5" customWidth="1"/>
-    <col min="3080" max="3080" width="20.33203125" customWidth="1"/>
-    <col min="3081" max="3081" width="14.83203125" customWidth="1"/>
-    <col min="3082" max="3082" width="12.1640625" customWidth="1"/>
-    <col min="3083" max="3083" width="18.6640625" customWidth="1"/>
-    <col min="3084" max="3084" width="8.83203125" customWidth="1"/>
-    <col min="3087" max="3087" width="12.83203125" customWidth="1"/>
-    <col min="3088" max="3088" width="36.33203125" customWidth="1"/>
-    <col min="3329" max="3329" width="8.1640625" customWidth="1"/>
+    <col min="3075" max="3075" width="11.453125" customWidth="1"/>
+    <col min="3076" max="3076" width="9.453125" customWidth="1"/>
+    <col min="3077" max="3077" width="7.36328125" customWidth="1"/>
+    <col min="3078" max="3078" width="6.453125" customWidth="1"/>
+    <col min="3079" max="3079" width="10.453125" customWidth="1"/>
+    <col min="3080" max="3080" width="20.36328125" customWidth="1"/>
+    <col min="3081" max="3081" width="14.81640625" customWidth="1"/>
+    <col min="3082" max="3082" width="12.1796875" customWidth="1"/>
+    <col min="3083" max="3083" width="18.6328125" customWidth="1"/>
+    <col min="3084" max="3084" width="8.81640625" customWidth="1"/>
+    <col min="3087" max="3087" width="12.81640625" customWidth="1"/>
+    <col min="3088" max="3088" width="36.36328125" customWidth="1"/>
+    <col min="3329" max="3329" width="8.1796875" customWidth="1"/>
     <col min="3330" max="3330" width="13" customWidth="1"/>
-    <col min="3331" max="3331" width="11.5" customWidth="1"/>
-    <col min="3332" max="3332" width="9.5" customWidth="1"/>
-    <col min="3333" max="3333" width="7.33203125" customWidth="1"/>
-    <col min="3334" max="3334" width="6.5" customWidth="1"/>
-    <col min="3335" max="3335" width="10.5" customWidth="1"/>
-    <col min="3336" max="3336" width="20.33203125" customWidth="1"/>
-    <col min="3337" max="3337" width="14.83203125" customWidth="1"/>
-    <col min="3338" max="3338" width="12.1640625" customWidth="1"/>
-    <col min="3339" max="3339" width="18.6640625" customWidth="1"/>
-    <col min="3340" max="3340" width="8.83203125" customWidth="1"/>
-    <col min="3343" max="3343" width="12.83203125" customWidth="1"/>
-    <col min="3344" max="3344" width="36.33203125" customWidth="1"/>
-    <col min="3585" max="3585" width="8.1640625" customWidth="1"/>
+    <col min="3331" max="3331" width="11.453125" customWidth="1"/>
+    <col min="3332" max="3332" width="9.453125" customWidth="1"/>
+    <col min="3333" max="3333" width="7.36328125" customWidth="1"/>
+    <col min="3334" max="3334" width="6.453125" customWidth="1"/>
+    <col min="3335" max="3335" width="10.453125" customWidth="1"/>
+    <col min="3336" max="3336" width="20.36328125" customWidth="1"/>
+    <col min="3337" max="3337" width="14.81640625" customWidth="1"/>
+    <col min="3338" max="3338" width="12.1796875" customWidth="1"/>
+    <col min="3339" max="3339" width="18.6328125" customWidth="1"/>
+    <col min="3340" max="3340" width="8.81640625" customWidth="1"/>
+    <col min="3343" max="3343" width="12.81640625" customWidth="1"/>
+    <col min="3344" max="3344" width="36.36328125" customWidth="1"/>
+    <col min="3585" max="3585" width="8.1796875" customWidth="1"/>
     <col min="3586" max="3586" width="13" customWidth="1"/>
-    <col min="3587" max="3587" width="11.5" customWidth="1"/>
-    <col min="3588" max="3588" width="9.5" customWidth="1"/>
-    <col min="3589" max="3589" width="7.33203125" customWidth="1"/>
-    <col min="3590" max="3590" width="6.5" customWidth="1"/>
-    <col min="3591" max="3591" width="10.5" customWidth="1"/>
-    <col min="3592" max="3592" width="20.33203125" customWidth="1"/>
-    <col min="3593" max="3593" width="14.83203125" customWidth="1"/>
-    <col min="3594" max="3594" width="12.1640625" customWidth="1"/>
-    <col min="3595" max="3595" width="18.6640625" customWidth="1"/>
-    <col min="3596" max="3596" width="8.83203125" customWidth="1"/>
-    <col min="3599" max="3599" width="12.83203125" customWidth="1"/>
-    <col min="3600" max="3600" width="36.33203125" customWidth="1"/>
-    <col min="3841" max="3841" width="8.1640625" customWidth="1"/>
+    <col min="3587" max="3587" width="11.453125" customWidth="1"/>
+    <col min="3588" max="3588" width="9.453125" customWidth="1"/>
+    <col min="3589" max="3589" width="7.36328125" customWidth="1"/>
+    <col min="3590" max="3590" width="6.453125" customWidth="1"/>
+    <col min="3591" max="3591" width="10.453125" customWidth="1"/>
+    <col min="3592" max="3592" width="20.36328125" customWidth="1"/>
+    <col min="3593" max="3593" width="14.81640625" customWidth="1"/>
+    <col min="3594" max="3594" width="12.1796875" customWidth="1"/>
+    <col min="3595" max="3595" width="18.6328125" customWidth="1"/>
+    <col min="3596" max="3596" width="8.81640625" customWidth="1"/>
+    <col min="3599" max="3599" width="12.81640625" customWidth="1"/>
+    <col min="3600" max="3600" width="36.36328125" customWidth="1"/>
+    <col min="3841" max="3841" width="8.1796875" customWidth="1"/>
     <col min="3842" max="3842" width="13" customWidth="1"/>
-    <col min="3843" max="3843" width="11.5" customWidth="1"/>
-    <col min="3844" max="3844" width="9.5" customWidth="1"/>
-    <col min="3845" max="3845" width="7.33203125" customWidth="1"/>
-    <col min="3846" max="3846" width="6.5" customWidth="1"/>
-    <col min="3847" max="3847" width="10.5" customWidth="1"/>
-    <col min="3848" max="3848" width="20.33203125" customWidth="1"/>
-    <col min="3849" max="3849" width="14.83203125" customWidth="1"/>
-    <col min="3850" max="3850" width="12.1640625" customWidth="1"/>
-    <col min="3851" max="3851" width="18.6640625" customWidth="1"/>
-    <col min="3852" max="3852" width="8.83203125" customWidth="1"/>
-    <col min="3855" max="3855" width="12.83203125" customWidth="1"/>
-    <col min="3856" max="3856" width="36.33203125" customWidth="1"/>
-    <col min="4097" max="4097" width="8.1640625" customWidth="1"/>
+    <col min="3843" max="3843" width="11.453125" customWidth="1"/>
+    <col min="3844" max="3844" width="9.453125" customWidth="1"/>
+    <col min="3845" max="3845" width="7.36328125" customWidth="1"/>
+    <col min="3846" max="3846" width="6.453125" customWidth="1"/>
+    <col min="3847" max="3847" width="10.453125" customWidth="1"/>
+    <col min="3848" max="3848" width="20.36328125" customWidth="1"/>
+    <col min="3849" max="3849" width="14.81640625" customWidth="1"/>
+    <col min="3850" max="3850" width="12.1796875" customWidth="1"/>
+    <col min="3851" max="3851" width="18.6328125" customWidth="1"/>
+    <col min="3852" max="3852" width="8.81640625" customWidth="1"/>
+    <col min="3855" max="3855" width="12.81640625" customWidth="1"/>
+    <col min="3856" max="3856" width="36.36328125" customWidth="1"/>
+    <col min="4097" max="4097" width="8.1796875" customWidth="1"/>
     <col min="4098" max="4098" width="13" customWidth="1"/>
-    <col min="4099" max="4099" width="11.5" customWidth="1"/>
-    <col min="4100" max="4100" width="9.5" customWidth="1"/>
-    <col min="4101" max="4101" width="7.33203125" customWidth="1"/>
-    <col min="4102" max="4102" width="6.5" customWidth="1"/>
-    <col min="4103" max="4103" width="10.5" customWidth="1"/>
-    <col min="4104" max="4104" width="20.33203125" customWidth="1"/>
-    <col min="4105" max="4105" width="14.83203125" customWidth="1"/>
-    <col min="4106" max="4106" width="12.1640625" customWidth="1"/>
-    <col min="4107" max="4107" width="18.6640625" customWidth="1"/>
-    <col min="4108" max="4108" width="8.83203125" customWidth="1"/>
-    <col min="4111" max="4111" width="12.83203125" customWidth="1"/>
-    <col min="4112" max="4112" width="36.33203125" customWidth="1"/>
-    <col min="4353" max="4353" width="8.1640625" customWidth="1"/>
+    <col min="4099" max="4099" width="11.453125" customWidth="1"/>
+    <col min="4100" max="4100" width="9.453125" customWidth="1"/>
+    <col min="4101" max="4101" width="7.36328125" customWidth="1"/>
+    <col min="4102" max="4102" width="6.453125" customWidth="1"/>
+    <col min="4103" max="4103" width="10.453125" customWidth="1"/>
+    <col min="4104" max="4104" width="20.36328125" customWidth="1"/>
+    <col min="4105" max="4105" width="14.81640625" customWidth="1"/>
+    <col min="4106" max="4106" width="12.1796875" customWidth="1"/>
+    <col min="4107" max="4107" width="18.6328125" customWidth="1"/>
+    <col min="4108" max="4108" width="8.81640625" customWidth="1"/>
+    <col min="4111" max="4111" width="12.81640625" customWidth="1"/>
+    <col min="4112" max="4112" width="36.36328125" customWidth="1"/>
+    <col min="4353" max="4353" width="8.1796875" customWidth="1"/>
     <col min="4354" max="4354" width="13" customWidth="1"/>
-    <col min="4355" max="4355" width="11.5" customWidth="1"/>
-    <col min="4356" max="4356" width="9.5" customWidth="1"/>
-    <col min="4357" max="4357" width="7.33203125" customWidth="1"/>
-    <col min="4358" max="4358" width="6.5" customWidth="1"/>
-    <col min="4359" max="4359" width="10.5" customWidth="1"/>
-    <col min="4360" max="4360" width="20.33203125" customWidth="1"/>
-    <col min="4361" max="4361" width="14.83203125" customWidth="1"/>
-    <col min="4362" max="4362" width="12.1640625" customWidth="1"/>
-    <col min="4363" max="4363" width="18.6640625" customWidth="1"/>
-    <col min="4364" max="4364" width="8.83203125" customWidth="1"/>
-    <col min="4367" max="4367" width="12.83203125" customWidth="1"/>
-    <col min="4368" max="4368" width="36.33203125" customWidth="1"/>
-    <col min="4609" max="4609" width="8.1640625" customWidth="1"/>
+    <col min="4355" max="4355" width="11.453125" customWidth="1"/>
+    <col min="4356" max="4356" width="9.453125" customWidth="1"/>
+    <col min="4357" max="4357" width="7.36328125" customWidth="1"/>
+    <col min="4358" max="4358" width="6.453125" customWidth="1"/>
+    <col min="4359" max="4359" width="10.453125" customWidth="1"/>
+    <col min="4360" max="4360" width="20.36328125" customWidth="1"/>
+    <col min="4361" max="4361" width="14.81640625" customWidth="1"/>
+    <col min="4362" max="4362" width="12.1796875" customWidth="1"/>
+    <col min="4363" max="4363" width="18.6328125" customWidth="1"/>
+    <col min="4364" max="4364" width="8.81640625" customWidth="1"/>
+    <col min="4367" max="4367" width="12.81640625" customWidth="1"/>
+    <col min="4368" max="4368" width="36.36328125" customWidth="1"/>
+    <col min="4609" max="4609" width="8.1796875" customWidth="1"/>
     <col min="4610" max="4610" width="13" customWidth="1"/>
-    <col min="4611" max="4611" width="11.5" customWidth="1"/>
-    <col min="4612" max="4612" width="9.5" customWidth="1"/>
-    <col min="4613" max="4613" width="7.33203125" customWidth="1"/>
-    <col min="4614" max="4614" width="6.5" customWidth="1"/>
-    <col min="4615" max="4615" width="10.5" customWidth="1"/>
-    <col min="4616" max="4616" width="20.33203125" customWidth="1"/>
-    <col min="4617" max="4617" width="14.83203125" customWidth="1"/>
-    <col min="4618" max="4618" width="12.1640625" customWidth="1"/>
-    <col min="4619" max="4619" width="18.6640625" customWidth="1"/>
-    <col min="4620" max="4620" width="8.83203125" customWidth="1"/>
-    <col min="4623" max="4623" width="12.83203125" customWidth="1"/>
-    <col min="4624" max="4624" width="36.33203125" customWidth="1"/>
-    <col min="4865" max="4865" width="8.1640625" customWidth="1"/>
+    <col min="4611" max="4611" width="11.453125" customWidth="1"/>
+    <col min="4612" max="4612" width="9.453125" customWidth="1"/>
+    <col min="4613" max="4613" width="7.36328125" customWidth="1"/>
+    <col min="4614" max="4614" width="6.453125" customWidth="1"/>
+    <col min="4615" max="4615" width="10.453125" customWidth="1"/>
+    <col min="4616" max="4616" width="20.36328125" customWidth="1"/>
+    <col min="4617" max="4617" width="14.81640625" customWidth="1"/>
+    <col min="4618" max="4618" width="12.1796875" customWidth="1"/>
+    <col min="4619" max="4619" width="18.6328125" customWidth="1"/>
+    <col min="4620" max="4620" width="8.81640625" customWidth="1"/>
+    <col min="4623" max="4623" width="12.81640625" customWidth="1"/>
+    <col min="4624" max="4624" width="36.36328125" customWidth="1"/>
+    <col min="4865" max="4865" width="8.1796875" customWidth="1"/>
     <col min="4866" max="4866" width="13" customWidth="1"/>
-    <col min="4867" max="4867" width="11.5" customWidth="1"/>
-    <col min="4868" max="4868" width="9.5" customWidth="1"/>
-    <col min="4869" max="4869" width="7.33203125" customWidth="1"/>
-    <col min="4870" max="4870" width="6.5" customWidth="1"/>
-    <col min="4871" max="4871" width="10.5" customWidth="1"/>
-    <col min="4872" max="4872" width="20.33203125" customWidth="1"/>
-    <col min="4873" max="4873" width="14.83203125" customWidth="1"/>
-    <col min="4874" max="4874" width="12.1640625" customWidth="1"/>
-    <col min="4875" max="4875" width="18.6640625" customWidth="1"/>
-    <col min="4876" max="4876" width="8.83203125" customWidth="1"/>
-    <col min="4879" max="4879" width="12.83203125" customWidth="1"/>
-    <col min="4880" max="4880" width="36.33203125" customWidth="1"/>
-    <col min="5121" max="5121" width="8.1640625" customWidth="1"/>
+    <col min="4867" max="4867" width="11.453125" customWidth="1"/>
+    <col min="4868" max="4868" width="9.453125" customWidth="1"/>
+    <col min="4869" max="4869" width="7.36328125" customWidth="1"/>
+    <col min="4870" max="4870" width="6.453125" customWidth="1"/>
+    <col min="4871" max="4871" width="10.453125" customWidth="1"/>
+    <col min="4872" max="4872" width="20.36328125" customWidth="1"/>
+    <col min="4873" max="4873" width="14.81640625" customWidth="1"/>
+    <col min="4874" max="4874" width="12.1796875" customWidth="1"/>
+    <col min="4875" max="4875" width="18.6328125" customWidth="1"/>
+    <col min="4876" max="4876" width="8.81640625" customWidth="1"/>
+    <col min="4879" max="4879" width="12.81640625" customWidth="1"/>
+    <col min="4880" max="4880" width="36.36328125" customWidth="1"/>
+    <col min="5121" max="5121" width="8.1796875" customWidth="1"/>
     <col min="5122" max="5122" width="13" customWidth="1"/>
-    <col min="5123" max="5123" width="11.5" customWidth="1"/>
-    <col min="5124" max="5124" width="9.5" customWidth="1"/>
-    <col min="5125" max="5125" width="7.33203125" customWidth="1"/>
-    <col min="5126" max="5126" width="6.5" customWidth="1"/>
-    <col min="5127" max="5127" width="10.5" customWidth="1"/>
-    <col min="5128" max="5128" width="20.33203125" customWidth="1"/>
-    <col min="5129" max="5129" width="14.83203125" customWidth="1"/>
-    <col min="5130" max="5130" width="12.1640625" customWidth="1"/>
-    <col min="5131" max="5131" width="18.6640625" customWidth="1"/>
-    <col min="5132" max="5132" width="8.83203125" customWidth="1"/>
-    <col min="5135" max="5135" width="12.83203125" customWidth="1"/>
-    <col min="5136" max="5136" width="36.33203125" customWidth="1"/>
-    <col min="5377" max="5377" width="8.1640625" customWidth="1"/>
+    <col min="5123" max="5123" width="11.453125" customWidth="1"/>
+    <col min="5124" max="5124" width="9.453125" customWidth="1"/>
+    <col min="5125" max="5125" width="7.36328125" customWidth="1"/>
+    <col min="5126" max="5126" width="6.453125" customWidth="1"/>
+    <col min="5127" max="5127" width="10.453125" customWidth="1"/>
+    <col min="5128" max="5128" width="20.36328125" customWidth="1"/>
+    <col min="5129" max="5129" width="14.81640625" customWidth="1"/>
+    <col min="5130" max="5130" width="12.1796875" customWidth="1"/>
+    <col min="5131" max="5131" width="18.6328125" customWidth="1"/>
+    <col min="5132" max="5132" width="8.81640625" customWidth="1"/>
+    <col min="5135" max="5135" width="12.81640625" customWidth="1"/>
+    <col min="5136" max="5136" width="36.36328125" customWidth="1"/>
+    <col min="5377" max="5377" width="8.1796875" customWidth="1"/>
     <col min="5378" max="5378" width="13" customWidth="1"/>
-    <col min="5379" max="5379" width="11.5" customWidth="1"/>
-    <col min="5380" max="5380" width="9.5" customWidth="1"/>
-    <col min="5381" max="5381" width="7.33203125" customWidth="1"/>
-    <col min="5382" max="5382" width="6.5" customWidth="1"/>
-    <col min="5383" max="5383" width="10.5" customWidth="1"/>
-    <col min="5384" max="5384" width="20.33203125" customWidth="1"/>
-    <col min="5385" max="5385" width="14.83203125" customWidth="1"/>
-    <col min="5386" max="5386" width="12.1640625" customWidth="1"/>
-    <col min="5387" max="5387" width="18.6640625" customWidth="1"/>
-    <col min="5388" max="5388" width="8.83203125" customWidth="1"/>
-    <col min="5391" max="5391" width="12.83203125" customWidth="1"/>
-    <col min="5392" max="5392" width="36.33203125" customWidth="1"/>
-    <col min="5633" max="5633" width="8.1640625" customWidth="1"/>
+    <col min="5379" max="5379" width="11.453125" customWidth="1"/>
+    <col min="5380" max="5380" width="9.453125" customWidth="1"/>
+    <col min="5381" max="5381" width="7.36328125" customWidth="1"/>
+    <col min="5382" max="5382" width="6.453125" customWidth="1"/>
+    <col min="5383" max="5383" width="10.453125" customWidth="1"/>
+    <col min="5384" max="5384" width="20.36328125" customWidth="1"/>
+    <col min="5385" max="5385" width="14.81640625" customWidth="1"/>
+    <col min="5386" max="5386" width="12.1796875" customWidth="1"/>
+    <col min="5387" max="5387" width="18.6328125" customWidth="1"/>
+    <col min="5388" max="5388" width="8.81640625" customWidth="1"/>
+    <col min="5391" max="5391" width="12.81640625" customWidth="1"/>
+    <col min="5392" max="5392" width="36.36328125" customWidth="1"/>
+    <col min="5633" max="5633" width="8.1796875" customWidth="1"/>
     <col min="5634" max="5634" width="13" customWidth="1"/>
-    <col min="5635" max="5635" width="11.5" customWidth="1"/>
-    <col min="5636" max="5636" width="9.5" customWidth="1"/>
-    <col min="5637" max="5637" width="7.33203125" customWidth="1"/>
-    <col min="5638" max="5638" width="6.5" customWidth="1"/>
-    <col min="5639" max="5639" width="10.5" customWidth="1"/>
-    <col min="5640" max="5640" width="20.33203125" customWidth="1"/>
-    <col min="5641" max="5641" width="14.83203125" customWidth="1"/>
-    <col min="5642" max="5642" width="12.1640625" customWidth="1"/>
-    <col min="5643" max="5643" width="18.6640625" customWidth="1"/>
-    <col min="5644" max="5644" width="8.83203125" customWidth="1"/>
-    <col min="5647" max="5647" width="12.83203125" customWidth="1"/>
-    <col min="5648" max="5648" width="36.33203125" customWidth="1"/>
-    <col min="5889" max="5889" width="8.1640625" customWidth="1"/>
+    <col min="5635" max="5635" width="11.453125" customWidth="1"/>
+    <col min="5636" max="5636" width="9.453125" customWidth="1"/>
+    <col min="5637" max="5637" width="7.36328125" customWidth="1"/>
+    <col min="5638" max="5638" width="6.453125" customWidth="1"/>
+    <col min="5639" max="5639" width="10.453125" customWidth="1"/>
+    <col min="5640" max="5640" width="20.36328125" customWidth="1"/>
+    <col min="5641" max="5641" width="14.81640625" customWidth="1"/>
+    <col min="5642" max="5642" width="12.1796875" customWidth="1"/>
+    <col min="5643" max="5643" width="18.6328125" customWidth="1"/>
+    <col min="5644" max="5644" width="8.81640625" customWidth="1"/>
+    <col min="5647" max="5647" width="12.81640625" customWidth="1"/>
+    <col min="5648" max="5648" width="36.36328125" customWidth="1"/>
+    <col min="5889" max="5889" width="8.1796875" customWidth="1"/>
     <col min="5890" max="5890" width="13" customWidth="1"/>
-    <col min="5891" max="5891" width="11.5" customWidth="1"/>
-    <col min="5892" max="5892" width="9.5" customWidth="1"/>
-    <col min="5893" max="5893" width="7.33203125" customWidth="1"/>
-    <col min="5894" max="5894" width="6.5" customWidth="1"/>
-    <col min="5895" max="5895" width="10.5" customWidth="1"/>
-    <col min="5896" max="5896" width="20.33203125" customWidth="1"/>
-    <col min="5897" max="5897" width="14.83203125" customWidth="1"/>
-    <col min="5898" max="5898" width="12.1640625" customWidth="1"/>
-    <col min="5899" max="5899" width="18.6640625" customWidth="1"/>
-    <col min="5900" max="5900" width="8.83203125" customWidth="1"/>
-    <col min="5903" max="5903" width="12.83203125" customWidth="1"/>
-    <col min="5904" max="5904" width="36.33203125" customWidth="1"/>
-    <col min="6145" max="6145" width="8.1640625" customWidth="1"/>
+    <col min="5891" max="5891" width="11.453125" customWidth="1"/>
+    <col min="5892" max="5892" width="9.453125" customWidth="1"/>
+    <col min="5893" max="5893" width="7.36328125" customWidth="1"/>
+    <col min="5894" max="5894" width="6.453125" customWidth="1"/>
+    <col min="5895" max="5895" width="10.453125" customWidth="1"/>
+    <col min="5896" max="5896" width="20.36328125" customWidth="1"/>
+    <col min="5897" max="5897" width="14.81640625" customWidth="1"/>
+    <col min="5898" max="5898" width="12.1796875" customWidth="1"/>
+    <col min="5899" max="5899" width="18.6328125" customWidth="1"/>
+    <col min="5900" max="5900" width="8.81640625" customWidth="1"/>
+    <col min="5903" max="5903" width="12.81640625" customWidth="1"/>
+    <col min="5904" max="5904" width="36.36328125" customWidth="1"/>
+    <col min="6145" max="6145" width="8.1796875" customWidth="1"/>
     <col min="6146" max="6146" width="13" customWidth="1"/>
-    <col min="6147" max="6147" width="11.5" customWidth="1"/>
-    <col min="6148" max="6148" width="9.5" customWidth="1"/>
-    <col min="6149" max="6149" width="7.33203125" customWidth="1"/>
-    <col min="6150" max="6150" width="6.5" customWidth="1"/>
-    <col min="6151" max="6151" width="10.5" customWidth="1"/>
-    <col min="6152" max="6152" width="20.33203125" customWidth="1"/>
-    <col min="6153" max="6153" width="14.83203125" customWidth="1"/>
-    <col min="6154" max="6154" width="12.1640625" customWidth="1"/>
-    <col min="6155" max="6155" width="18.6640625" customWidth="1"/>
-    <col min="6156" max="6156" width="8.83203125" customWidth="1"/>
-    <col min="6159" max="6159" width="12.83203125" customWidth="1"/>
-    <col min="6160" max="6160" width="36.33203125" customWidth="1"/>
-    <col min="6401" max="6401" width="8.1640625" customWidth="1"/>
+    <col min="6147" max="6147" width="11.453125" customWidth="1"/>
+    <col min="6148" max="6148" width="9.453125" customWidth="1"/>
+    <col min="6149" max="6149" width="7.36328125" customWidth="1"/>
+    <col min="6150" max="6150" width="6.453125" customWidth="1"/>
+    <col min="6151" max="6151" width="10.453125" customWidth="1"/>
+    <col min="6152" max="6152" width="20.36328125" customWidth="1"/>
+    <col min="6153" max="6153" width="14.81640625" customWidth="1"/>
+    <col min="6154" max="6154" width="12.1796875" customWidth="1"/>
+    <col min="6155" max="6155" width="18.6328125" customWidth="1"/>
+    <col min="6156" max="6156" width="8.81640625" customWidth="1"/>
+    <col min="6159" max="6159" width="12.81640625" customWidth="1"/>
+    <col min="6160" max="6160" width="36.36328125" customWidth="1"/>
+    <col min="6401" max="6401" width="8.1796875" customWidth="1"/>
     <col min="6402" max="6402" width="13" customWidth="1"/>
-    <col min="6403" max="6403" width="11.5" customWidth="1"/>
-    <col min="6404" max="6404" width="9.5" customWidth="1"/>
-    <col min="6405" max="6405" width="7.33203125" customWidth="1"/>
-    <col min="6406" max="6406" width="6.5" customWidth="1"/>
-    <col min="6407" max="6407" width="10.5" customWidth="1"/>
-    <col min="6408" max="6408" width="20.33203125" customWidth="1"/>
-    <col min="6409" max="6409" width="14.83203125" customWidth="1"/>
-    <col min="6410" max="6410" width="12.1640625" customWidth="1"/>
-    <col min="6411" max="6411" width="18.6640625" customWidth="1"/>
-    <col min="6412" max="6412" width="8.83203125" customWidth="1"/>
-    <col min="6415" max="6415" width="12.83203125" customWidth="1"/>
-    <col min="6416" max="6416" width="36.33203125" customWidth="1"/>
-    <col min="6657" max="6657" width="8.1640625" customWidth="1"/>
+    <col min="6403" max="6403" width="11.453125" customWidth="1"/>
+    <col min="6404" max="6404" width="9.453125" customWidth="1"/>
+    <col min="6405" max="6405" width="7.36328125" customWidth="1"/>
+    <col min="6406" max="6406" width="6.453125" customWidth="1"/>
+    <col min="6407" max="6407" width="10.453125" customWidth="1"/>
+    <col min="6408" max="6408" width="20.36328125" customWidth="1"/>
+    <col min="6409" max="6409" width="14.81640625" customWidth="1"/>
+    <col min="6410" max="6410" width="12.1796875" customWidth="1"/>
+    <col min="6411" max="6411" width="18.6328125" customWidth="1"/>
+    <col min="6412" max="6412" width="8.81640625" customWidth="1"/>
+    <col min="6415" max="6415" width="12.81640625" customWidth="1"/>
+    <col min="6416" max="6416" width="36.36328125" customWidth="1"/>
+    <col min="6657" max="6657" width="8.1796875" customWidth="1"/>
     <col min="6658" max="6658" width="13" customWidth="1"/>
-    <col min="6659" max="6659" width="11.5" customWidth="1"/>
-    <col min="6660" max="6660" width="9.5" customWidth="1"/>
-    <col min="6661" max="6661" width="7.33203125" customWidth="1"/>
-    <col min="6662" max="6662" width="6.5" customWidth="1"/>
-    <col min="6663" max="6663" width="10.5" customWidth="1"/>
-    <col min="6664" max="6664" width="20.33203125" customWidth="1"/>
-    <col min="6665" max="6665" width="14.83203125" customWidth="1"/>
-    <col min="6666" max="6666" width="12.1640625" customWidth="1"/>
-    <col min="6667" max="6667" width="18.6640625" customWidth="1"/>
-    <col min="6668" max="6668" width="8.83203125" customWidth="1"/>
-    <col min="6671" max="6671" width="12.83203125" customWidth="1"/>
-    <col min="6672" max="6672" width="36.33203125" customWidth="1"/>
-    <col min="6913" max="6913" width="8.1640625" customWidth="1"/>
+    <col min="6659" max="6659" width="11.453125" customWidth="1"/>
+    <col min="6660" max="6660" width="9.453125" customWidth="1"/>
+    <col min="6661" max="6661" width="7.36328125" customWidth="1"/>
+    <col min="6662" max="6662" width="6.453125" customWidth="1"/>
+    <col min="6663" max="6663" width="10.453125" customWidth="1"/>
+    <col min="6664" max="6664" width="20.36328125" customWidth="1"/>
+    <col min="6665" max="6665" width="14.81640625" customWidth="1"/>
+    <col min="6666" max="6666" width="12.1796875" customWidth="1"/>
+    <col min="6667" max="6667" width="18.6328125" customWidth="1"/>
+    <col min="6668" max="6668" width="8.81640625" customWidth="1"/>
+    <col min="6671" max="6671" width="12.81640625" customWidth="1"/>
+    <col min="6672" max="6672" width="36.36328125" customWidth="1"/>
+    <col min="6913" max="6913" width="8.1796875" customWidth="1"/>
     <col min="6914" max="6914" width="13" customWidth="1"/>
-    <col min="6915" max="6915" width="11.5" customWidth="1"/>
-    <col min="6916" max="6916" width="9.5" customWidth="1"/>
-    <col min="6917" max="6917" width="7.33203125" customWidth="1"/>
-    <col min="6918" max="6918" width="6.5" customWidth="1"/>
-    <col min="6919" max="6919" width="10.5" customWidth="1"/>
-    <col min="6920" max="6920" width="20.33203125" customWidth="1"/>
-    <col min="6921" max="6921" width="14.83203125" customWidth="1"/>
-    <col min="6922" max="6922" width="12.1640625" customWidth="1"/>
-    <col min="6923" max="6923" width="18.6640625" customWidth="1"/>
-    <col min="6924" max="6924" width="8.83203125" customWidth="1"/>
-    <col min="6927" max="6927" width="12.83203125" customWidth="1"/>
-    <col min="6928" max="6928" width="36.33203125" customWidth="1"/>
-    <col min="7169" max="7169" width="8.1640625" customWidth="1"/>
+    <col min="6915" max="6915" width="11.453125" customWidth="1"/>
+    <col min="6916" max="6916" width="9.453125" customWidth="1"/>
+    <col min="6917" max="6917" width="7.36328125" customWidth="1"/>
+    <col min="6918" max="6918" width="6.453125" customWidth="1"/>
+    <col min="6919" max="6919" width="10.453125" customWidth="1"/>
+    <col min="6920" max="6920" width="20.36328125" customWidth="1"/>
+    <col min="6921" max="6921" width="14.81640625" customWidth="1"/>
+    <col min="6922" max="6922" width="12.1796875" customWidth="1"/>
+    <col min="6923" max="6923" width="18.6328125" customWidth="1"/>
+    <col min="6924" max="6924" width="8.81640625" customWidth="1"/>
+    <col min="6927" max="6927" width="12.81640625" customWidth="1"/>
+    <col min="6928" max="6928" width="36.36328125" customWidth="1"/>
+    <col min="7169" max="7169" width="8.1796875" customWidth="1"/>
     <col min="7170" max="7170" width="13" customWidth="1"/>
-    <col min="7171" max="7171" width="11.5" customWidth="1"/>
-    <col min="7172" max="7172" width="9.5" customWidth="1"/>
-    <col min="7173" max="7173" width="7.33203125" customWidth="1"/>
-    <col min="7174" max="7174" width="6.5" customWidth="1"/>
-    <col min="7175" max="7175" width="10.5" customWidth="1"/>
-    <col min="7176" max="7176" width="20.33203125" customWidth="1"/>
-    <col min="7177" max="7177" width="14.83203125" customWidth="1"/>
-    <col min="7178" max="7178" width="12.1640625" customWidth="1"/>
-    <col min="7179" max="7179" width="18.6640625" customWidth="1"/>
-    <col min="7180" max="7180" width="8.83203125" customWidth="1"/>
-    <col min="7183" max="7183" width="12.83203125" customWidth="1"/>
-    <col min="7184" max="7184" width="36.33203125" customWidth="1"/>
-    <col min="7425" max="7425" width="8.1640625" customWidth="1"/>
+    <col min="7171" max="7171" width="11.453125" customWidth="1"/>
+    <col min="7172" max="7172" width="9.453125" customWidth="1"/>
+    <col min="7173" max="7173" width="7.36328125" customWidth="1"/>
+    <col min="7174" max="7174" width="6.453125" customWidth="1"/>
+    <col min="7175" max="7175" width="10.453125" customWidth="1"/>
+    <col min="7176" max="7176" width="20.36328125" customWidth="1"/>
+    <col min="7177" max="7177" width="14.81640625" customWidth="1"/>
+    <col min="7178" max="7178" width="12.1796875" customWidth="1"/>
+    <col min="7179" max="7179" width="18.6328125" customWidth="1"/>
+    <col min="7180" max="7180" width="8.81640625" customWidth="1"/>
+    <col min="7183" max="7183" width="12.81640625" customWidth="1"/>
+    <col min="7184" max="7184" width="36.36328125" customWidth="1"/>
+    <col min="7425" max="7425" width="8.1796875" customWidth="1"/>
     <col min="7426" max="7426" width="13" customWidth="1"/>
-    <col min="7427" max="7427" width="11.5" customWidth="1"/>
-    <col min="7428" max="7428" width="9.5" customWidth="1"/>
-    <col min="7429" max="7429" width="7.33203125" customWidth="1"/>
-    <col min="7430" max="7430" width="6.5" customWidth="1"/>
-    <col min="7431" max="7431" width="10.5" customWidth="1"/>
-    <col min="7432" max="7432" width="20.33203125" customWidth="1"/>
-    <col min="7433" max="7433" width="14.83203125" customWidth="1"/>
-    <col min="7434" max="7434" width="12.1640625" customWidth="1"/>
-    <col min="7435" max="7435" width="18.6640625" customWidth="1"/>
-    <col min="7436" max="7436" width="8.83203125" customWidth="1"/>
-    <col min="7439" max="7439" width="12.83203125" customWidth="1"/>
-    <col min="7440" max="7440" width="36.33203125" customWidth="1"/>
-    <col min="7681" max="7681" width="8.1640625" customWidth="1"/>
+    <col min="7427" max="7427" width="11.453125" customWidth="1"/>
+    <col min="7428" max="7428" width="9.453125" customWidth="1"/>
+    <col min="7429" max="7429" width="7.36328125" customWidth="1"/>
+    <col min="7430" max="7430" width="6.453125" customWidth="1"/>
+    <col min="7431" max="7431" width="10.453125" customWidth="1"/>
+    <col min="7432" max="7432" width="20.36328125" customWidth="1"/>
+    <col min="7433" max="7433" width="14.81640625" customWidth="1"/>
+    <col min="7434" max="7434" width="12.1796875" customWidth="1"/>
+    <col min="7435" max="7435" width="18.6328125" customWidth="1"/>
+    <col min="7436" max="7436" width="8.81640625" customWidth="1"/>
+    <col min="7439" max="7439" width="12.81640625" customWidth="1"/>
+    <col min="7440" max="7440" width="36.36328125" customWidth="1"/>
+    <col min="7681" max="7681" width="8.1796875" customWidth="1"/>
     <col min="7682" max="7682" width="13" customWidth="1"/>
-    <col min="7683" max="7683" width="11.5" customWidth="1"/>
-    <col min="7684" max="7684" width="9.5" customWidth="1"/>
-    <col min="7685" max="7685" width="7.33203125" customWidth="1"/>
-    <col min="7686" max="7686" width="6.5" customWidth="1"/>
-    <col min="7687" max="7687" width="10.5" customWidth="1"/>
-    <col min="7688" max="7688" width="20.33203125" customWidth="1"/>
-    <col min="7689" max="7689" width="14.83203125" customWidth="1"/>
-    <col min="7690" max="7690" width="12.1640625" customWidth="1"/>
-    <col min="7691" max="7691" width="18.6640625" customWidth="1"/>
-    <col min="7692" max="7692" width="8.83203125" customWidth="1"/>
-    <col min="7695" max="7695" width="12.83203125" customWidth="1"/>
-    <col min="7696" max="7696" width="36.33203125" customWidth="1"/>
-    <col min="7937" max="7937" width="8.1640625" customWidth="1"/>
+    <col min="7683" max="7683" width="11.453125" customWidth="1"/>
+    <col min="7684" max="7684" width="9.453125" customWidth="1"/>
+    <col min="7685" max="7685" width="7.36328125" customWidth="1"/>
+    <col min="7686" max="7686" width="6.453125" customWidth="1"/>
+    <col min="7687" max="7687" width="10.453125" customWidth="1"/>
+    <col min="7688" max="7688" width="20.36328125" customWidth="1"/>
+    <col min="7689" max="7689" width="14.81640625" customWidth="1"/>
+    <col min="7690" max="7690" width="12.1796875" customWidth="1"/>
+    <col min="7691" max="7691" width="18.6328125" customWidth="1"/>
+    <col min="7692" max="7692" width="8.81640625" customWidth="1"/>
+    <col min="7695" max="7695" width="12.81640625" customWidth="1"/>
+    <col min="7696" max="7696" width="36.36328125" customWidth="1"/>
+    <col min="7937" max="7937" width="8.1796875" customWidth="1"/>
     <col min="7938" max="7938" width="13" customWidth="1"/>
-    <col min="7939" max="7939" width="11.5" customWidth="1"/>
-    <col min="7940" max="7940" width="9.5" customWidth="1"/>
-    <col min="7941" max="7941" width="7.33203125" customWidth="1"/>
-    <col min="7942" max="7942" width="6.5" customWidth="1"/>
-    <col min="7943" max="7943" width="10.5" customWidth="1"/>
-    <col min="7944" max="7944" width="20.33203125" customWidth="1"/>
-    <col min="7945" max="7945" width="14.83203125" customWidth="1"/>
-    <col min="7946" max="7946" width="12.1640625" customWidth="1"/>
-    <col min="7947" max="7947" width="18.6640625" customWidth="1"/>
-    <col min="7948" max="7948" width="8.83203125" customWidth="1"/>
-    <col min="7951" max="7951" width="12.83203125" customWidth="1"/>
-    <col min="7952" max="7952" width="36.33203125" customWidth="1"/>
-    <col min="8193" max="8193" width="8.1640625" customWidth="1"/>
+    <col min="7939" max="7939" width="11.453125" customWidth="1"/>
+    <col min="7940" max="7940" width="9.453125" customWidth="1"/>
+    <col min="7941" max="7941" width="7.36328125" customWidth="1"/>
+    <col min="7942" max="7942" width="6.453125" customWidth="1"/>
+    <col min="7943" max="7943" width="10.453125" customWidth="1"/>
+    <col min="7944" max="7944" width="20.36328125" customWidth="1"/>
+    <col min="7945" max="7945" width="14.81640625" customWidth="1"/>
+    <col min="7946" max="7946" width="12.1796875" customWidth="1"/>
+    <col min="7947" max="7947" width="18.6328125" customWidth="1"/>
+    <col min="7948" max="7948" width="8.81640625" customWidth="1"/>
+    <col min="7951" max="7951" width="12.81640625" customWidth="1"/>
+    <col min="7952" max="7952" width="36.36328125" customWidth="1"/>
+    <col min="8193" max="8193" width="8.1796875" customWidth="1"/>
     <col min="8194" max="8194" width="13" customWidth="1"/>
-    <col min="8195" max="8195" width="11.5" customWidth="1"/>
-    <col min="8196" max="8196" width="9.5" customWidth="1"/>
-    <col min="8197" max="8197" width="7.33203125" customWidth="1"/>
-    <col min="8198" max="8198" width="6.5" customWidth="1"/>
-    <col min="8199" max="8199" width="10.5" customWidth="1"/>
-    <col min="8200" max="8200" width="20.33203125" customWidth="1"/>
-    <col min="8201" max="8201" width="14.83203125" customWidth="1"/>
-    <col min="8202" max="8202" width="12.1640625" customWidth="1"/>
-    <col min="8203" max="8203" width="18.6640625" customWidth="1"/>
-    <col min="8204" max="8204" width="8.83203125" customWidth="1"/>
-    <col min="8207" max="8207" width="12.83203125" customWidth="1"/>
-    <col min="8208" max="8208" width="36.33203125" customWidth="1"/>
-    <col min="8449" max="8449" width="8.1640625" customWidth="1"/>
+    <col min="8195" max="8195" width="11.453125" customWidth="1"/>
+    <col min="8196" max="8196" width="9.453125" customWidth="1"/>
+    <col min="8197" max="8197" width="7.36328125" customWidth="1"/>
+    <col min="8198" max="8198" width="6.453125" customWidth="1"/>
+    <col min="8199" max="8199" width="10.453125" customWidth="1"/>
+    <col min="8200" max="8200" width="20.36328125" customWidth="1"/>
+    <col min="8201" max="8201" width="14.81640625" customWidth="1"/>
+    <col min="8202" max="8202" width="12.1796875" customWidth="1"/>
+    <col min="8203" max="8203" width="18.6328125" customWidth="1"/>
+    <col min="8204" max="8204" width="8.81640625" customWidth="1"/>
+    <col min="8207" max="8207" width="12.81640625" customWidth="1"/>
+    <col min="8208" max="8208" width="36.36328125" customWidth="1"/>
+    <col min="8449" max="8449" width="8.1796875" customWidth="1"/>
     <col min="8450" max="8450" width="13" customWidth="1"/>
-    <col min="8451" max="8451" width="11.5" customWidth="1"/>
-    <col min="8452" max="8452" width="9.5" customWidth="1"/>
-    <col min="8453" max="8453" width="7.33203125" customWidth="1"/>
-    <col min="8454" max="8454" width="6.5" customWidth="1"/>
-    <col min="8455" max="8455" width="10.5" customWidth="1"/>
-    <col min="8456" max="8456" width="20.33203125" customWidth="1"/>
-    <col min="8457" max="8457" width="14.83203125" customWidth="1"/>
-    <col min="8458" max="8458" width="12.1640625" customWidth="1"/>
-    <col min="8459" max="8459" width="18.6640625" customWidth="1"/>
-    <col min="8460" max="8460" width="8.83203125" customWidth="1"/>
-    <col min="8463" max="8463" width="12.83203125" customWidth="1"/>
-    <col min="8464" max="8464" width="36.33203125" customWidth="1"/>
-    <col min="8705" max="8705" width="8.1640625" customWidth="1"/>
+    <col min="8451" max="8451" width="11.453125" customWidth="1"/>
+    <col min="8452" max="8452" width="9.453125" customWidth="1"/>
+    <col min="8453" max="8453" width="7.36328125" customWidth="1"/>
+    <col min="8454" max="8454" width="6.453125" customWidth="1"/>
+    <col min="8455" max="8455" width="10.453125" customWidth="1"/>
+    <col min="8456" max="8456" width="20.36328125" customWidth="1"/>
+    <col min="8457" max="8457" width="14.81640625" customWidth="1"/>
+    <col min="8458" max="8458" width="12.1796875" customWidth="1"/>
+    <col min="8459" max="8459" width="18.6328125" customWidth="1"/>
+    <col min="8460" max="8460" width="8.81640625" customWidth="1"/>
+    <col min="8463" max="8463" width="12.81640625" customWidth="1"/>
+    <col min="8464" max="8464" width="36.36328125" customWidth="1"/>
+    <col min="8705" max="8705" width="8.1796875" customWidth="1"/>
     <col min="8706" max="8706" width="13" customWidth="1"/>
-    <col min="8707" max="8707" width="11.5" customWidth="1"/>
-    <col min="8708" max="8708" width="9.5" customWidth="1"/>
-    <col min="8709" max="8709" width="7.33203125" customWidth="1"/>
-    <col min="8710" max="8710" width="6.5" customWidth="1"/>
-    <col min="8711" max="8711" width="10.5" customWidth="1"/>
-    <col min="8712" max="8712" width="20.33203125" customWidth="1"/>
-    <col min="8713" max="8713" width="14.83203125" customWidth="1"/>
-    <col min="8714" max="8714" width="12.1640625" customWidth="1"/>
-    <col min="8715" max="8715" width="18.6640625" customWidth="1"/>
-    <col min="8716" max="8716" width="8.83203125" customWidth="1"/>
-    <col min="8719" max="8719" width="12.83203125" customWidth="1"/>
-    <col min="8720" max="8720" width="36.33203125" customWidth="1"/>
-    <col min="8961" max="8961" width="8.1640625" customWidth="1"/>
+    <col min="8707" max="8707" width="11.453125" customWidth="1"/>
+    <col min="8708" max="8708" width="9.453125" customWidth="1"/>
+    <col min="8709" max="8709" width="7.36328125" customWidth="1"/>
+    <col min="8710" max="8710" width="6.453125" customWidth="1"/>
+    <col min="8711" max="8711" width="10.453125" customWidth="1"/>
+    <col min="8712" max="8712" width="20.36328125" customWidth="1"/>
+    <col min="8713" max="8713" width="14.81640625" customWidth="1"/>
+    <col min="8714" max="8714" width="12.1796875" customWidth="1"/>
+    <col min="8715" max="8715" width="18.6328125" customWidth="1"/>
+    <col min="8716" max="8716" width="8.81640625" customWidth="1"/>
+    <col min="8719" max="8719" width="12.81640625" customWidth="1"/>
+    <col min="8720" max="8720" width="36.36328125" customWidth="1"/>
+    <col min="8961" max="8961" width="8.1796875" customWidth="1"/>
     <col min="8962" max="8962" width="13" customWidth="1"/>
-    <col min="8963" max="8963" width="11.5" customWidth="1"/>
-    <col min="8964" max="8964" width="9.5" customWidth="1"/>
-    <col min="8965" max="8965" width="7.33203125" customWidth="1"/>
-    <col min="8966" max="8966" width="6.5" customWidth="1"/>
-    <col min="8967" max="8967" width="10.5" customWidth="1"/>
-    <col min="8968" max="8968" width="20.33203125" customWidth="1"/>
-    <col min="8969" max="8969" width="14.83203125" customWidth="1"/>
-    <col min="8970" max="8970" width="12.1640625" customWidth="1"/>
-    <col min="8971" max="8971" width="18.6640625" customWidth="1"/>
-    <col min="8972" max="8972" width="8.83203125" customWidth="1"/>
-    <col min="8975" max="8975" width="12.83203125" customWidth="1"/>
-    <col min="8976" max="8976" width="36.33203125" customWidth="1"/>
-    <col min="9217" max="9217" width="8.1640625" customWidth="1"/>
+    <col min="8963" max="8963" width="11.453125" customWidth="1"/>
+    <col min="8964" max="8964" width="9.453125" customWidth="1"/>
+    <col min="8965" max="8965" width="7.36328125" customWidth="1"/>
+    <col min="8966" max="8966" width="6.453125" customWidth="1"/>
+    <col min="8967" max="8967" width="10.453125" customWidth="1"/>
+    <col min="8968" max="8968" width="20.36328125" customWidth="1"/>
+    <col min="8969" max="8969" width="14.81640625" customWidth="1"/>
+    <col min="8970" max="8970" width="12.1796875" customWidth="1"/>
+    <col min="8971" max="8971" width="18.6328125" customWidth="1"/>
+    <col min="8972" max="8972" width="8.81640625" customWidth="1"/>
+    <col min="8975" max="8975" width="12.81640625" customWidth="1"/>
+    <col min="8976" max="8976" width="36.36328125" customWidth="1"/>
+    <col min="9217" max="9217" width="8.1796875" customWidth="1"/>
     <col min="9218" max="9218" width="13" customWidth="1"/>
-    <col min="9219" max="9219" width="11.5" customWidth="1"/>
-    <col min="9220" max="9220" width="9.5" customWidth="1"/>
-    <col min="9221" max="9221" width="7.33203125" customWidth="1"/>
-    <col min="9222" max="9222" width="6.5" customWidth="1"/>
-    <col min="9223" max="9223" width="10.5" customWidth="1"/>
-    <col min="9224" max="9224" width="20.33203125" customWidth="1"/>
-    <col min="9225" max="9225" width="14.83203125" customWidth="1"/>
-    <col min="9226" max="9226" width="12.1640625" customWidth="1"/>
-    <col min="9227" max="9227" width="18.6640625" customWidth="1"/>
-    <col min="9228" max="9228" width="8.83203125" customWidth="1"/>
-    <col min="9231" max="9231" width="12.83203125" customWidth="1"/>
-    <col min="9232" max="9232" width="36.33203125" customWidth="1"/>
-    <col min="9473" max="9473" width="8.1640625" customWidth="1"/>
+    <col min="9219" max="9219" width="11.453125" customWidth="1"/>
+    <col min="9220" max="9220" width="9.453125" customWidth="1"/>
+    <col min="9221" max="9221" width="7.36328125" customWidth="1"/>
+    <col min="9222" max="9222" width="6.453125" customWidth="1"/>
+    <col min="9223" max="9223" width="10.453125" customWidth="1"/>
+    <col min="9224" max="9224" width="20.36328125" customWidth="1"/>
+    <col min="9225" max="9225" width="14.81640625" customWidth="1"/>
+    <col min="9226" max="9226" width="12.1796875" customWidth="1"/>
+    <col min="9227" max="9227" width="18.6328125" customWidth="1"/>
+    <col min="9228" max="9228" width="8.81640625" customWidth="1"/>
+    <col min="9231" max="9231" width="12.81640625" customWidth="1"/>
+    <col min="9232" max="9232" width="36.36328125" customWidth="1"/>
+    <col min="9473" max="9473" width="8.1796875" customWidth="1"/>
     <col min="9474" max="9474" width="13" customWidth="1"/>
-    <col min="9475" max="9475" width="11.5" customWidth="1"/>
-    <col min="9476" max="9476" width="9.5" customWidth="1"/>
-    <col min="9477" max="9477" width="7.33203125" customWidth="1"/>
-    <col min="9478" max="9478" width="6.5" customWidth="1"/>
-    <col min="9479" max="9479" width="10.5" customWidth="1"/>
-    <col min="9480" max="9480" width="20.33203125" customWidth="1"/>
-    <col min="9481" max="9481" width="14.83203125" customWidth="1"/>
-    <col min="9482" max="9482" width="12.1640625" customWidth="1"/>
-    <col min="9483" max="9483" width="18.6640625" customWidth="1"/>
-    <col min="9484" max="9484" width="8.83203125" customWidth="1"/>
-    <col min="9487" max="9487" width="12.83203125" customWidth="1"/>
-    <col min="9488" max="9488" width="36.33203125" customWidth="1"/>
-    <col min="9729" max="9729" width="8.1640625" customWidth="1"/>
+    <col min="9475" max="9475" width="11.453125" customWidth="1"/>
+    <col min="9476" max="9476" width="9.453125" customWidth="1"/>
+    <col min="9477" max="9477" width="7.36328125" customWidth="1"/>
+    <col min="9478" max="9478" width="6.453125" customWidth="1"/>
+    <col min="9479" max="9479" width="10.453125" customWidth="1"/>
+    <col min="9480" max="9480" width="20.36328125" customWidth="1"/>
+    <col min="9481" max="9481" width="14.81640625" customWidth="1"/>
+    <col min="9482" max="9482" width="12.1796875" customWidth="1"/>
+    <col min="9483" max="9483" width="18.6328125" customWidth="1"/>
+    <col min="9484" max="9484" width="8.81640625" customWidth="1"/>
+    <col min="9487" max="9487" width="12.81640625" customWidth="1"/>
+    <col min="9488" max="9488" width="36.36328125" customWidth="1"/>
+    <col min="9729" max="9729" width="8.1796875" customWidth="1"/>
     <col min="9730" max="9730" width="13" customWidth="1"/>
-    <col min="9731" max="9731" width="11.5" customWidth="1"/>
-    <col min="9732" max="9732" width="9.5" customWidth="1"/>
-    <col min="9733" max="9733" width="7.33203125" customWidth="1"/>
-    <col min="9734" max="9734" width="6.5" customWidth="1"/>
-    <col min="9735" max="9735" width="10.5" customWidth="1"/>
-    <col min="9736" max="9736" width="20.33203125" customWidth="1"/>
-    <col min="9737" max="9737" width="14.83203125" customWidth="1"/>
-    <col min="9738" max="9738" width="12.1640625" customWidth="1"/>
-    <col min="9739" max="9739" width="18.6640625" customWidth="1"/>
-    <col min="9740" max="9740" width="8.83203125" customWidth="1"/>
-    <col min="9743" max="9743" width="12.83203125" customWidth="1"/>
-    <col min="9744" max="9744" width="36.33203125" customWidth="1"/>
-    <col min="9985" max="9985" width="8.1640625" customWidth="1"/>
+    <col min="9731" max="9731" width="11.453125" customWidth="1"/>
+    <col min="9732" max="9732" width="9.453125" customWidth="1"/>
+    <col min="9733" max="9733" width="7.36328125" customWidth="1"/>
+    <col min="9734" max="9734" width="6.453125" customWidth="1"/>
+    <col min="9735" max="9735" width="10.453125" customWidth="1"/>
+    <col min="9736" max="9736" width="20.36328125" customWidth="1"/>
+    <col min="9737" max="9737" width="14.81640625" customWidth="1"/>
+    <col min="9738" max="9738" width="12.1796875" customWidth="1"/>
+    <col min="9739" max="9739" width="18.6328125" customWidth="1"/>
+    <col min="9740" max="9740" width="8.81640625" customWidth="1"/>
+    <col min="9743" max="9743" width="12.81640625" customWidth="1"/>
+    <col min="9744" max="9744" width="36.36328125" customWidth="1"/>
+    <col min="9985" max="9985" width="8.1796875" customWidth="1"/>
     <col min="9986" max="9986" width="13" customWidth="1"/>
-    <col min="9987" max="9987" width="11.5" customWidth="1"/>
-    <col min="9988" max="9988" width="9.5" customWidth="1"/>
-    <col min="9989" max="9989" width="7.33203125" customWidth="1"/>
-    <col min="9990" max="9990" width="6.5" customWidth="1"/>
-    <col min="9991" max="9991" width="10.5" customWidth="1"/>
-    <col min="9992" max="9992" width="20.33203125" customWidth="1"/>
-    <col min="9993" max="9993" width="14.83203125" customWidth="1"/>
-    <col min="9994" max="9994" width="12.1640625" customWidth="1"/>
-    <col min="9995" max="9995" width="18.6640625" customWidth="1"/>
-    <col min="9996" max="9996" width="8.83203125" customWidth="1"/>
-    <col min="9999" max="9999" width="12.83203125" customWidth="1"/>
-    <col min="10000" max="10000" width="36.33203125" customWidth="1"/>
-    <col min="10241" max="10241" width="8.1640625" customWidth="1"/>
+    <col min="9987" max="9987" width="11.453125" customWidth="1"/>
+    <col min="9988" max="9988" width="9.453125" customWidth="1"/>
+    <col min="9989" max="9989" width="7.36328125" customWidth="1"/>
+    <col min="9990" max="9990" width="6.453125" customWidth="1"/>
+    <col min="9991" max="9991" width="10.453125" customWidth="1"/>
+    <col min="9992" max="9992" width="20.36328125" customWidth="1"/>
+    <col min="9993" max="9993" width="14.81640625" customWidth="1"/>
+    <col min="9994" max="9994" width="12.1796875" customWidth="1"/>
+    <col min="9995" max="9995" width="18.6328125" customWidth="1"/>
+    <col min="9996" max="9996" width="8.81640625" customWidth="1"/>
+    <col min="9999" max="9999" width="12.81640625" customWidth="1"/>
+    <col min="10000" max="10000" width="36.36328125" customWidth="1"/>
+    <col min="10241" max="10241" width="8.1796875" customWidth="1"/>
     <col min="10242" max="10242" width="13" customWidth="1"/>
-    <col min="10243" max="10243" width="11.5" customWidth="1"/>
-    <col min="10244" max="10244" width="9.5" customWidth="1"/>
-    <col min="10245" max="10245" width="7.33203125" customWidth="1"/>
-    <col min="10246" max="10246" width="6.5" customWidth="1"/>
-    <col min="10247" max="10247" width="10.5" customWidth="1"/>
-    <col min="10248" max="10248" width="20.33203125" customWidth="1"/>
-    <col min="10249" max="10249" width="14.83203125" customWidth="1"/>
-    <col min="10250" max="10250" width="12.1640625" customWidth="1"/>
-    <col min="10251" max="10251" width="18.6640625" customWidth="1"/>
-    <col min="10252" max="10252" width="8.83203125" customWidth="1"/>
-    <col min="10255" max="10255" width="12.83203125" customWidth="1"/>
-    <col min="10256" max="10256" width="36.33203125" customWidth="1"/>
-    <col min="10497" max="10497" width="8.1640625" customWidth="1"/>
+    <col min="10243" max="10243" width="11.453125" customWidth="1"/>
+    <col min="10244" max="10244" width="9.453125" customWidth="1"/>
+    <col min="10245" max="10245" width="7.36328125" customWidth="1"/>
+    <col min="10246" max="10246" width="6.453125" customWidth="1"/>
+    <col min="10247" max="10247" width="10.453125" customWidth="1"/>
+    <col min="10248" max="10248" width="20.36328125" customWidth="1"/>
+    <col min="10249" max="10249" width="14.81640625" customWidth="1"/>
+    <col min="10250" max="10250" width="12.1796875" customWidth="1"/>
+    <col min="10251" max="10251" width="18.6328125" customWidth="1"/>
+    <col min="10252" max="10252" width="8.81640625" customWidth="1"/>
+    <col min="10255" max="10255" width="12.81640625" customWidth="1"/>
+    <col min="10256" max="10256" width="36.36328125" customWidth="1"/>
+    <col min="10497" max="10497" width="8.1796875" customWidth="1"/>
     <col min="10498" max="10498" width="13" customWidth="1"/>
-    <col min="10499" max="10499" width="11.5" customWidth="1"/>
-    <col min="10500" max="10500" width="9.5" customWidth="1"/>
-    <col min="10501" max="10501" width="7.33203125" customWidth="1"/>
-    <col min="10502" max="10502" width="6.5" customWidth="1"/>
-    <col min="10503" max="10503" width="10.5" customWidth="1"/>
-    <col min="10504" max="10504" width="20.33203125" customWidth="1"/>
-    <col min="10505" max="10505" width="14.83203125" customWidth="1"/>
-    <col min="10506" max="10506" width="12.1640625" customWidth="1"/>
-    <col min="10507" max="10507" width="18.6640625" customWidth="1"/>
-    <col min="10508" max="10508" width="8.83203125" customWidth="1"/>
-    <col min="10511" max="10511" width="12.83203125" customWidth="1"/>
-    <col min="10512" max="10512" width="36.33203125" customWidth="1"/>
-    <col min="10753" max="10753" width="8.1640625" customWidth="1"/>
+    <col min="10499" max="10499" width="11.453125" customWidth="1"/>
+    <col min="10500" max="10500" width="9.453125" customWidth="1"/>
+    <col min="10501" max="10501" width="7.36328125" customWidth="1"/>
+    <col min="10502" max="10502" width="6.453125" customWidth="1"/>
+    <col min="10503" max="10503" width="10.453125" customWidth="1"/>
+    <col min="10504" max="10504" width="20.36328125" customWidth="1"/>
+    <col min="10505" max="10505" width="14.81640625" customWidth="1"/>
+    <col min="10506" max="10506" width="12.1796875" customWidth="1"/>
+    <col min="10507" max="10507" width="18.6328125" customWidth="1"/>
+    <col min="10508" max="10508" width="8.81640625" customWidth="1"/>
+    <col min="10511" max="10511" width="12.81640625" customWidth="1"/>
+    <col min="10512" max="10512" width="36.36328125" customWidth="1"/>
+    <col min="10753" max="10753" width="8.1796875" customWidth="1"/>
     <col min="10754" max="10754" width="13" customWidth="1"/>
-    <col min="10755" max="10755" width="11.5" customWidth="1"/>
-    <col min="10756" max="10756" width="9.5" customWidth="1"/>
-    <col min="10757" max="10757" width="7.33203125" customWidth="1"/>
-    <col min="10758" max="10758" width="6.5" customWidth="1"/>
-    <col min="10759" max="10759" width="10.5" customWidth="1"/>
-    <col min="10760" max="10760" width="20.33203125" customWidth="1"/>
-    <col min="10761" max="10761" width="14.83203125" customWidth="1"/>
-    <col min="10762" max="10762" width="12.1640625" customWidth="1"/>
-    <col min="10763" max="10763" width="18.6640625" customWidth="1"/>
-    <col min="10764" max="10764" width="8.83203125" customWidth="1"/>
-    <col min="10767" max="10767" width="12.83203125" customWidth="1"/>
-    <col min="10768" max="10768" width="36.33203125" customWidth="1"/>
-    <col min="11009" max="11009" width="8.1640625" customWidth="1"/>
+    <col min="10755" max="10755" width="11.453125" customWidth="1"/>
+    <col min="10756" max="10756" width="9.453125" customWidth="1"/>
+    <col min="10757" max="10757" width="7.36328125" customWidth="1"/>
+    <col min="10758" max="10758" width="6.453125" customWidth="1"/>
+    <col min="10759" max="10759" width="10.453125" customWidth="1"/>
+    <col min="10760" max="10760" width="20.36328125" customWidth="1"/>
+    <col min="10761" max="10761" width="14.81640625" customWidth="1"/>
+    <col min="10762" max="10762" width="12.1796875" customWidth="1"/>
+    <col min="10763" max="10763" width="18.6328125" customWidth="1"/>
+    <col min="10764" max="10764" width="8.81640625" customWidth="1"/>
+    <col min="10767" max="10767" width="12.81640625" customWidth="1"/>
+    <col min="10768" max="10768" width="36.36328125" customWidth="1"/>
+    <col min="11009" max="11009" width="8.1796875" customWidth="1"/>
     <col min="11010" max="11010" width="13" customWidth="1"/>
-    <col min="11011" max="11011" width="11.5" customWidth="1"/>
-    <col min="11012" max="11012" width="9.5" customWidth="1"/>
-    <col min="11013" max="11013" width="7.33203125" customWidth="1"/>
-    <col min="11014" max="11014" width="6.5" customWidth="1"/>
-    <col min="11015" max="11015" width="10.5" customWidth="1"/>
-    <col min="11016" max="11016" width="20.33203125" customWidth="1"/>
-    <col min="11017" max="11017" width="14.83203125" customWidth="1"/>
-    <col min="11018" max="11018" width="12.1640625" customWidth="1"/>
-    <col min="11019" max="11019" width="18.6640625" customWidth="1"/>
-    <col min="11020" max="11020" width="8.83203125" customWidth="1"/>
-    <col min="11023" max="11023" width="12.83203125" customWidth="1"/>
-    <col min="11024" max="11024" width="36.33203125" customWidth="1"/>
-    <col min="11265" max="11265" width="8.1640625" customWidth="1"/>
+    <col min="11011" max="11011" width="11.453125" customWidth="1"/>
+    <col min="11012" max="11012" width="9.453125" customWidth="1"/>
+    <col min="11013" max="11013" width="7.36328125" customWidth="1"/>
+    <col min="11014" max="11014" width="6.453125" customWidth="1"/>
+    <col min="11015" max="11015" width="10.453125" customWidth="1"/>
+    <col min="11016" max="11016" width="20.36328125" customWidth="1"/>
+    <col min="11017" max="11017" width="14.81640625" customWidth="1"/>
+    <col min="11018" max="11018" width="12.1796875" customWidth="1"/>
+    <col min="11019" max="11019" width="18.6328125" customWidth="1"/>
+    <col min="11020" max="11020" width="8.81640625" customWidth="1"/>
+    <col min="11023" max="11023" width="12.81640625" customWidth="1"/>
+    <col min="11024" max="11024" width="36.36328125" customWidth="1"/>
+    <col min="11265" max="11265" width="8.1796875" customWidth="1"/>
     <col min="11266" max="11266" width="13" customWidth="1"/>
-    <col min="11267" max="11267" width="11.5" customWidth="1"/>
-    <col min="11268" max="11268" width="9.5" customWidth="1"/>
-    <col min="11269" max="11269" width="7.33203125" customWidth="1"/>
-    <col min="11270" max="11270" width="6.5" customWidth="1"/>
-    <col min="11271" max="11271" width="10.5" customWidth="1"/>
-    <col min="11272" max="11272" width="20.33203125" customWidth="1"/>
-    <col min="11273" max="11273" width="14.83203125" customWidth="1"/>
-    <col min="11274" max="11274" width="12.1640625" customWidth="1"/>
-    <col min="11275" max="11275" width="18.6640625" customWidth="1"/>
-    <col min="11276" max="11276" width="8.83203125" customWidth="1"/>
-    <col min="11279" max="11279" width="12.83203125" customWidth="1"/>
-    <col min="11280" max="11280" width="36.33203125" customWidth="1"/>
-    <col min="11521" max="11521" width="8.1640625" customWidth="1"/>
+    <col min="11267" max="11267" width="11.453125" customWidth="1"/>
+    <col min="11268" max="11268" width="9.453125" customWidth="1"/>
+    <col min="11269" max="11269" width="7.36328125" customWidth="1"/>
+    <col min="11270" max="11270" width="6.453125" customWidth="1"/>
+    <col min="11271" max="11271" width="10.453125" customWidth="1"/>
+    <col min="11272" max="11272" width="20.36328125" customWidth="1"/>
+    <col min="11273" max="11273" width="14.81640625" customWidth="1"/>
+    <col min="11274" max="11274" width="12.1796875" customWidth="1"/>
+    <col min="11275" max="11275" width="18.6328125" customWidth="1"/>
+    <col min="11276" max="11276" width="8.81640625" customWidth="1"/>
+    <col min="11279" max="11279" width="12.81640625" customWidth="1"/>
+    <col min="11280" max="11280" width="36.36328125" customWidth="1"/>
+    <col min="11521" max="11521" width="8.1796875" customWidth="1"/>
     <col min="11522" max="11522" width="13" customWidth="1"/>
-    <col min="11523" max="11523" width="11.5" customWidth="1"/>
-    <col min="11524" max="11524" width="9.5" customWidth="1"/>
-    <col min="11525" max="11525" width="7.33203125" customWidth="1"/>
-    <col min="11526" max="11526" width="6.5" customWidth="1"/>
-    <col min="11527" max="11527" width="10.5" customWidth="1"/>
-    <col min="11528" max="11528" width="20.33203125" customWidth="1"/>
-    <col min="11529" max="11529" width="14.83203125" customWidth="1"/>
-    <col min="11530" max="11530" width="12.1640625" customWidth="1"/>
-    <col min="11531" max="11531" width="18.6640625" customWidth="1"/>
-    <col min="11532" max="11532" width="8.83203125" customWidth="1"/>
-    <col min="11535" max="11535" width="12.83203125" customWidth="1"/>
-    <col min="11536" max="11536" width="36.33203125" customWidth="1"/>
-    <col min="11777" max="11777" width="8.1640625" customWidth="1"/>
+    <col min="11523" max="11523" width="11.453125" customWidth="1"/>
+    <col min="11524" max="11524" width="9.453125" customWidth="1"/>
+    <col min="11525" max="11525" width="7.36328125" customWidth="1"/>
+    <col min="11526" max="11526" width="6.453125" customWidth="1"/>
+    <col min="11527" max="11527" width="10.453125" customWidth="1"/>
+    <col min="11528" max="11528" width="20.36328125" customWidth="1"/>
+    <col min="11529" max="11529" width="14.81640625" customWidth="1"/>
+    <col min="11530" max="11530" width="12.1796875" customWidth="1"/>
+    <col min="11531" max="11531" width="18.6328125" customWidth="1"/>
+    <col min="11532" max="11532" width="8.81640625" customWidth="1"/>
+    <col min="11535" max="11535" width="12.81640625" customWidth="1"/>
+    <col min="11536" max="11536" width="36.36328125" customWidth="1"/>
+    <col min="11777" max="11777" width="8.1796875" customWidth="1"/>
     <col min="11778" max="11778" width="13" customWidth="1"/>
-    <col min="11779" max="11779" width="11.5" customWidth="1"/>
-    <col min="11780" max="11780" width="9.5" customWidth="1"/>
-    <col min="11781" max="11781" width="7.33203125" customWidth="1"/>
-    <col min="11782" max="11782" width="6.5" customWidth="1"/>
-    <col min="11783" max="11783" width="10.5" customWidth="1"/>
-    <col min="11784" max="11784" width="20.33203125" customWidth="1"/>
-    <col min="11785" max="11785" width="14.83203125" customWidth="1"/>
-    <col min="11786" max="11786" width="12.1640625" customWidth="1"/>
-    <col min="11787" max="11787" width="18.6640625" customWidth="1"/>
-    <col min="11788" max="11788" width="8.83203125" customWidth="1"/>
-    <col min="11791" max="11791" width="12.83203125" customWidth="1"/>
-    <col min="11792" max="11792" width="36.33203125" customWidth="1"/>
-    <col min="12033" max="12033" width="8.1640625" customWidth="1"/>
+    <col min="11779" max="11779" width="11.453125" customWidth="1"/>
+    <col min="11780" max="11780" width="9.453125" customWidth="1"/>
+    <col min="11781" max="11781" width="7.36328125" customWidth="1"/>
+    <col min="11782" max="11782" width="6.453125" customWidth="1"/>
+    <col min="11783" max="11783" width="10.453125" customWidth="1"/>
+    <col min="11784" max="11784" width="20.36328125" customWidth="1"/>
+    <col min="11785" max="11785" width="14.81640625" customWidth="1"/>
+    <col min="11786" max="11786" width="12.1796875" customWidth="1"/>
+    <col min="11787" max="11787" width="18.6328125" customWidth="1"/>
+    <col min="11788" max="11788" width="8.81640625" customWidth="1"/>
+    <col min="11791" max="11791" width="12.81640625" customWidth="1"/>
+    <col min="11792" max="11792" width="36.36328125" customWidth="1"/>
+    <col min="12033" max="12033" width="8.1796875" customWidth="1"/>
     <col min="12034" max="12034" width="13" customWidth="1"/>
-    <col min="12035" max="12035" width="11.5" customWidth="1"/>
-    <col min="12036" max="12036" width="9.5" customWidth="1"/>
-    <col min="12037" max="12037" width="7.33203125" customWidth="1"/>
-    <col min="12038" max="12038" width="6.5" customWidth="1"/>
-    <col min="12039" max="12039" width="10.5" customWidth="1"/>
-    <col min="12040" max="12040" width="20.33203125" customWidth="1"/>
-    <col min="12041" max="12041" width="14.83203125" customWidth="1"/>
-    <col min="12042" max="12042" width="12.1640625" customWidth="1"/>
-    <col min="12043" max="12043" width="18.6640625" customWidth="1"/>
-    <col min="12044" max="12044" width="8.83203125" customWidth="1"/>
-    <col min="12047" max="12047" width="12.83203125" customWidth="1"/>
-    <col min="12048" max="12048" width="36.33203125" customWidth="1"/>
-    <col min="12289" max="12289" width="8.1640625" customWidth="1"/>
+    <col min="12035" max="12035" width="11.453125" customWidth="1"/>
+    <col min="12036" max="12036" width="9.453125" customWidth="1"/>
+    <col min="12037" max="12037" width="7.36328125" customWidth="1"/>
+    <col min="12038" max="12038" width="6.453125" customWidth="1"/>
+    <col min="12039" max="12039" width="10.453125" customWidth="1"/>
+    <col min="12040" max="12040" width="20.36328125" customWidth="1"/>
+    <col min="12041" max="12041" width="14.81640625" customWidth="1"/>
+    <col min="12042" max="12042" width="12.1796875" customWidth="1"/>
+    <col min="12043" max="12043" width="18.6328125" customWidth="1"/>
+    <col min="12044" max="12044" width="8.81640625" customWidth="1"/>
+    <col min="12047" max="12047" width="12.81640625" customWidth="1"/>
+    <col min="12048" max="12048" width="36.36328125" customWidth="1"/>
+    <col min="12289" max="12289" width="8.1796875" customWidth="1"/>
     <col min="12290" max="12290" width="13" customWidth="1"/>
-    <col min="12291" max="12291" width="11.5" customWidth="1"/>
-    <col min="12292" max="12292" width="9.5" customWidth="1"/>
-    <col min="12293" max="12293" width="7.33203125" customWidth="1"/>
-    <col min="12294" max="12294" width="6.5" customWidth="1"/>
-    <col min="12295" max="12295" width="10.5" customWidth="1"/>
-    <col min="12296" max="12296" width="20.33203125" customWidth="1"/>
-    <col min="12297" max="12297" width="14.83203125" customWidth="1"/>
-    <col min="12298" max="12298" width="12.1640625" customWidth="1"/>
-    <col min="12299" max="12299" width="18.6640625" customWidth="1"/>
-    <col min="12300" max="12300" width="8.83203125" customWidth="1"/>
-    <col min="12303" max="12303" width="12.83203125" customWidth="1"/>
-    <col min="12304" max="12304" width="36.33203125" customWidth="1"/>
-    <col min="12545" max="12545" width="8.1640625" customWidth="1"/>
+    <col min="12291" max="12291" width="11.453125" customWidth="1"/>
+    <col min="12292" max="12292" width="9.453125" customWidth="1"/>
+    <col min="12293" max="12293" width="7.36328125" customWidth="1"/>
+    <col min="12294" max="12294" width="6.453125" customWidth="1"/>
+    <col min="12295" max="12295" width="10.453125" customWidth="1"/>
+    <col min="12296" max="12296" width="20.36328125" customWidth="1"/>
+    <col min="12297" max="12297" width="14.81640625" customWidth="1"/>
+    <col min="12298" max="12298" width="12.1796875" customWidth="1"/>
+    <col min="12299" max="12299" width="18.6328125" customWidth="1"/>
+    <col min="12300" max="12300" width="8.81640625" customWidth="1"/>
+    <col min="12303" max="12303" width="12.81640625" customWidth="1"/>
+    <col min="12304" max="12304" width="36.36328125" customWidth="1"/>
+    <col min="12545" max="12545" width="8.1796875" customWidth="1"/>
     <col min="12546" max="12546" width="13" customWidth="1"/>
-    <col min="12547" max="12547" width="11.5" customWidth="1"/>
-    <col min="12548" max="12548" width="9.5" customWidth="1"/>
-    <col min="12549" max="12549" width="7.33203125" customWidth="1"/>
-    <col min="12550" max="12550" width="6.5" customWidth="1"/>
-    <col min="12551" max="12551" width="10.5" customWidth="1"/>
-    <col min="12552" max="12552" width="20.33203125" customWidth="1"/>
-    <col min="12553" max="12553" width="14.83203125" customWidth="1"/>
-    <col min="12554" max="12554" width="12.1640625" customWidth="1"/>
-    <col min="12555" max="12555" width="18.6640625" customWidth="1"/>
-    <col min="12556" max="12556" width="8.83203125" customWidth="1"/>
-    <col min="12559" max="12559" width="12.83203125" customWidth="1"/>
-    <col min="12560" max="12560" width="36.33203125" customWidth="1"/>
-    <col min="12801" max="12801" width="8.1640625" customWidth="1"/>
+    <col min="12547" max="12547" width="11.453125" customWidth="1"/>
+    <col min="12548" max="12548" width="9.453125" customWidth="1"/>
+    <col min="12549" max="12549" width="7.36328125" customWidth="1"/>
+    <col min="12550" max="12550" width="6.453125" customWidth="1"/>
+    <col min="12551" max="12551" width="10.453125" customWidth="1"/>
+    <col min="12552" max="12552" width="20.36328125" customWidth="1"/>
+    <col min="12553" max="12553" width="14.81640625" customWidth="1"/>
+    <col min="12554" max="12554" width="12.1796875" customWidth="1"/>
+    <col min="12555" max="12555" width="18.6328125" customWidth="1"/>
+    <col min="12556" max="12556" width="8.81640625" customWidth="1"/>
+    <col min="12559" max="12559" width="12.81640625" customWidth="1"/>
+    <col min="12560" max="12560" width="36.36328125" customWidth="1"/>
+    <col min="12801" max="12801" width="8.1796875" customWidth="1"/>
     <col min="12802" max="12802" width="13" customWidth="1"/>
-    <col min="12803" max="12803" width="11.5" customWidth="1"/>
-    <col min="12804" max="12804" width="9.5" customWidth="1"/>
-    <col min="12805" max="12805" width="7.33203125" customWidth="1"/>
-    <col min="12806" max="12806" width="6.5" customWidth="1"/>
-    <col min="12807" max="12807" width="10.5" customWidth="1"/>
-    <col min="12808" max="12808" width="20.33203125" customWidth="1"/>
-    <col min="12809" max="12809" width="14.83203125" customWidth="1"/>
-    <col min="12810" max="12810" width="12.1640625" customWidth="1"/>
-    <col min="12811" max="12811" width="18.6640625" customWidth="1"/>
-    <col min="12812" max="12812" width="8.83203125" customWidth="1"/>
-    <col min="12815" max="12815" width="12.83203125" customWidth="1"/>
-    <col min="12816" max="12816" width="36.33203125" customWidth="1"/>
-    <col min="13057" max="13057" width="8.1640625" customWidth="1"/>
+    <col min="12803" max="12803" width="11.453125" customWidth="1"/>
+    <col min="12804" max="12804" width="9.453125" customWidth="1"/>
+    <col min="12805" max="12805" width="7.36328125" customWidth="1"/>
+    <col min="12806" max="12806" width="6.453125" customWidth="1"/>
+    <col min="12807" max="12807" width="10.453125" customWidth="1"/>
+    <col min="12808" max="12808" width="20.36328125" customWidth="1"/>
+    <col min="12809" max="12809" width="14.81640625" customWidth="1"/>
+    <col min="12810" max="12810" width="12.1796875" customWidth="1"/>
+    <col min="12811" max="12811" width="18.6328125" customWidth="1"/>
+    <col min="12812" max="12812" width="8.81640625" customWidth="1"/>
+    <col min="12815" max="12815" width="12.81640625" customWidth="1"/>
+    <col min="12816" max="12816" width="36.36328125" customWidth="1"/>
+    <col min="13057" max="13057" width="8.1796875" customWidth="1"/>
     <col min="13058" max="13058" width="13" customWidth="1"/>
-    <col min="13059" max="13059" width="11.5" customWidth="1"/>
-    <col min="13060" max="13060" width="9.5" customWidth="1"/>
-    <col min="13061" max="13061" width="7.33203125" customWidth="1"/>
-    <col min="13062" max="13062" width="6.5" customWidth="1"/>
-    <col min="13063" max="13063" width="10.5" customWidth="1"/>
-    <col min="13064" max="13064" width="20.33203125" customWidth="1"/>
-    <col min="13065" max="13065" width="14.83203125" customWidth="1"/>
-    <col min="13066" max="13066" width="12.1640625" customWidth="1"/>
-    <col min="13067" max="13067" width="18.6640625" customWidth="1"/>
-    <col min="13068" max="13068" width="8.83203125" customWidth="1"/>
-    <col min="13071" max="13071" width="12.83203125" customWidth="1"/>
-    <col min="13072" max="13072" width="36.33203125" customWidth="1"/>
-    <col min="13313" max="13313" width="8.1640625" customWidth="1"/>
+    <col min="13059" max="13059" width="11.453125" customWidth="1"/>
+    <col min="13060" max="13060" width="9.453125" customWidth="1"/>
+    <col min="13061" max="13061" width="7.36328125" customWidth="1"/>
+    <col min="13062" max="13062" width="6.453125" customWidth="1"/>
+    <col min="13063" max="13063" width="10.453125" customWidth="1"/>
+    <col min="13064" max="13064" width="20.36328125" customWidth="1"/>
+    <col min="13065" max="13065" width="14.81640625" customWidth="1"/>
+    <col min="13066" max="13066" width="12.1796875" customWidth="1"/>
+    <col min="13067" max="13067" width="18.6328125" customWidth="1"/>
+    <col min="13068" max="13068" width="8.81640625" customWidth="1"/>
+    <col min="13071" max="13071" width="12.81640625" customWidth="1"/>
+    <col min="13072" max="13072" width="36.36328125" customWidth="1"/>
+    <col min="13313" max="13313" width="8.1796875" customWidth="1"/>
     <col min="13314" max="13314" width="13" customWidth="1"/>
-    <col min="13315" max="13315" width="11.5" customWidth="1"/>
-    <col min="13316" max="13316" width="9.5" customWidth="1"/>
-    <col min="13317" max="13317" width="7.33203125" customWidth="1"/>
-    <col min="13318" max="13318" width="6.5" customWidth="1"/>
-    <col min="13319" max="13319" width="10.5" customWidth="1"/>
-    <col min="13320" max="13320" width="20.33203125" customWidth="1"/>
-    <col min="13321" max="13321" width="14.83203125" customWidth="1"/>
-    <col min="13322" max="13322" width="12.1640625" customWidth="1"/>
-    <col min="13323" max="13323" width="18.6640625" customWidth="1"/>
-    <col min="13324" max="13324" width="8.83203125" customWidth="1"/>
-    <col min="13327" max="13327" width="12.83203125" customWidth="1"/>
-    <col min="13328" max="13328" width="36.33203125" customWidth="1"/>
-    <col min="13569" max="13569" width="8.1640625" customWidth="1"/>
+    <col min="13315" max="13315" width="11.453125" customWidth="1"/>
+    <col min="13316" max="13316" width="9.453125" customWidth="1"/>
+    <col min="13317" max="13317" width="7.36328125" customWidth="1"/>
+    <col min="13318" max="13318" width="6.453125" customWidth="1"/>
+    <col min="13319" max="13319" width="10.453125" customWidth="1"/>
+    <col min="13320" max="13320" width="20.36328125" customWidth="1"/>
+    <col min="13321" max="13321" width="14.81640625" customWidth="1"/>
+    <col min="13322" max="13322" width="12.1796875" customWidth="1"/>
+    <col min="13323" max="13323" width="18.6328125" customWidth="1"/>
+    <col min="13324" max="13324" width="8.81640625" customWidth="1"/>
+    <col min="13327" max="13327" width="12.81640625" customWidth="1"/>
+    <col min="13328" max="13328" width="36.36328125" customWidth="1"/>
+    <col min="13569" max="13569" width="8.1796875" customWidth="1"/>
     <col min="13570" max="13570" width="13" customWidth="1"/>
-    <col min="13571" max="13571" width="11.5" customWidth="1"/>
-    <col min="13572" max="13572" width="9.5" customWidth="1"/>
-    <col min="13573" max="13573" width="7.33203125" customWidth="1"/>
-    <col min="13574" max="13574" width="6.5" customWidth="1"/>
-    <col min="13575" max="13575" width="10.5" customWidth="1"/>
-    <col min="13576" max="13576" width="20.33203125" customWidth="1"/>
-    <col min="13577" max="13577" width="14.83203125" customWidth="1"/>
-    <col min="13578" max="13578" width="12.1640625" customWidth="1"/>
-    <col min="13579" max="13579" width="18.6640625" customWidth="1"/>
-    <col min="13580" max="13580" width="8.83203125" customWidth="1"/>
-    <col min="13583" max="13583" width="12.83203125" customWidth="1"/>
-    <col min="13584" max="13584" width="36.33203125" customWidth="1"/>
-    <col min="13825" max="13825" width="8.1640625" customWidth="1"/>
+    <col min="13571" max="13571" width="11.453125" customWidth="1"/>
+    <col min="13572" max="13572" width="9.453125" customWidth="1"/>
+    <col min="13573" max="13573" width="7.36328125" customWidth="1"/>
+    <col min="13574" max="13574" width="6.453125" customWidth="1"/>
+    <col min="13575" max="13575" width="10.453125" customWidth="1"/>
+    <col min="13576" max="13576" width="20.36328125" customWidth="1"/>
+    <col min="13577" max="13577" width="14.81640625" customWidth="1"/>
+    <col min="13578" max="13578" width="12.1796875" customWidth="1"/>
+    <col min="13579" max="13579" width="18.6328125" customWidth="1"/>
+    <col min="13580" max="13580" width="8.81640625" customWidth="1"/>
+    <col min="13583" max="13583" width="12.81640625" customWidth="1"/>
+    <col min="13584" max="13584" width="36.36328125" customWidth="1"/>
+    <col min="13825" max="13825" width="8.1796875" customWidth="1"/>
     <col min="13826" max="13826" width="13" customWidth="1"/>
-    <col min="13827" max="13827" width="11.5" customWidth="1"/>
-    <col min="13828" max="13828" width="9.5" customWidth="1"/>
-    <col min="13829" max="13829" width="7.33203125" customWidth="1"/>
-    <col min="13830" max="13830" width="6.5" customWidth="1"/>
-    <col min="13831" max="13831" width="10.5" customWidth="1"/>
-    <col min="13832" max="13832" width="20.33203125" customWidth="1"/>
-    <col min="13833" max="13833" width="14.83203125" customWidth="1"/>
-    <col min="13834" max="13834" width="12.1640625" customWidth="1"/>
-    <col min="13835" max="13835" width="18.6640625" customWidth="1"/>
-    <col min="13836" max="13836" width="8.83203125" customWidth="1"/>
-    <col min="13839" max="13839" width="12.83203125" customWidth="1"/>
-    <col min="13840" max="13840" width="36.33203125" customWidth="1"/>
-    <col min="14081" max="14081" width="8.1640625" customWidth="1"/>
+    <col min="13827" max="13827" width="11.453125" customWidth="1"/>
+    <col min="13828" max="13828" width="9.453125" customWidth="1"/>
+    <col min="13829" max="13829" width="7.36328125" customWidth="1"/>
+    <col min="13830" max="13830" width="6.453125" customWidth="1"/>
+    <col min="13831" max="13831" width="10.453125" customWidth="1"/>
+    <col min="13832" max="13832" width="20.36328125" customWidth="1"/>
+    <col min="13833" max="13833" width="14.81640625" customWidth="1"/>
+    <col min="13834" max="13834" width="12.1796875" customWidth="1"/>
+    <col min="13835" max="13835" width="18.6328125" customWidth="1"/>
+    <col min="13836" max="13836" width="8.81640625" customWidth="1"/>
+    <col min="13839" max="13839" width="12.81640625" customWidth="1"/>
+    <col min="13840" max="13840" width="36.36328125" customWidth="1"/>
+    <col min="14081" max="14081" width="8.1796875" customWidth="1"/>
     <col min="14082" max="14082" width="13" customWidth="1"/>
-    <col min="14083" max="14083" width="11.5" customWidth="1"/>
-    <col min="14084" max="14084" width="9.5" customWidth="1"/>
-    <col min="14085" max="14085" width="7.33203125" customWidth="1"/>
-    <col min="14086" max="14086" width="6.5" customWidth="1"/>
-    <col min="14087" max="14087" width="10.5" customWidth="1"/>
-    <col min="14088" max="14088" width="20.33203125" customWidth="1"/>
-    <col min="14089" max="14089" width="14.83203125" customWidth="1"/>
-    <col min="14090" max="14090" width="12.1640625" customWidth="1"/>
-    <col min="14091" max="14091" width="18.6640625" customWidth="1"/>
-    <col min="14092" max="14092" width="8.83203125" customWidth="1"/>
-    <col min="14095" max="14095" width="12.83203125" customWidth="1"/>
-    <col min="14096" max="14096" width="36.33203125" customWidth="1"/>
-    <col min="14337" max="14337" width="8.1640625" customWidth="1"/>
+    <col min="14083" max="14083" width="11.453125" customWidth="1"/>
+    <col min="14084" max="14084" width="9.453125" customWidth="1"/>
+    <col min="14085" max="14085" width="7.36328125" customWidth="1"/>
+    <col min="14086" max="14086" width="6.453125" customWidth="1"/>
+    <col min="14087" max="14087" width="10.453125" customWidth="1"/>
+    <col min="14088" max="14088" width="20.36328125" customWidth="1"/>
+    <col min="14089" max="14089" width="14.81640625" customWidth="1"/>
+    <col min="14090" max="14090" width="12.1796875" customWidth="1"/>
+    <col min="14091" max="14091" width="18.6328125" customWidth="1"/>
+    <col min="14092" max="14092" width="8.81640625" customWidth="1"/>
+    <col min="14095" max="14095" width="12.81640625" customWidth="1"/>
+    <col min="14096" max="14096" width="36.36328125" customWidth="1"/>
+    <col min="14337" max="14337" width="8.1796875" customWidth="1"/>
     <col min="14338" max="14338" width="13" customWidth="1"/>
-    <col min="14339" max="14339" width="11.5" customWidth="1"/>
-    <col min="14340" max="14340" width="9.5" customWidth="1"/>
-    <col min="14341" max="14341" width="7.33203125" customWidth="1"/>
-    <col min="14342" max="14342" width="6.5" customWidth="1"/>
-    <col min="14343" max="14343" width="10.5" customWidth="1"/>
-    <col min="14344" max="14344" width="20.33203125" customWidth="1"/>
-    <col min="14345" max="14345" width="14.83203125" customWidth="1"/>
-    <col min="14346" max="14346" width="12.1640625" customWidth="1"/>
-    <col min="14347" max="14347" width="18.6640625" customWidth="1"/>
-    <col min="14348" max="14348" width="8.83203125" customWidth="1"/>
-    <col min="14351" max="14351" width="12.83203125" customWidth="1"/>
-    <col min="14352" max="14352" width="36.33203125" customWidth="1"/>
-    <col min="14593" max="14593" width="8.1640625" customWidth="1"/>
+    <col min="14339" max="14339" width="11.453125" customWidth="1"/>
+    <col min="14340" max="14340" width="9.453125" customWidth="1"/>
+    <col min="14341" max="14341" width="7.36328125" customWidth="1"/>
+    <col min="14342" max="14342" width="6.453125" customWidth="1"/>
+    <col min="14343" max="14343" width="10.453125" customWidth="1"/>
+    <col min="14344" max="14344" width="20.36328125" customWidth="1"/>
+    <col min="14345" max="14345" width="14.81640625" customWidth="1"/>
+    <col min="14346" max="14346" width="12.1796875" customWidth="1"/>
+    <col min="14347" max="14347" width="18.6328125" customWidth="1"/>
+    <col min="14348" max="14348" width="8.81640625" customWidth="1"/>
+    <col min="14351" max="14351" width="12.81640625" customWidth="1"/>
+    <col min="14352" max="14352" width="36.36328125" customWidth="1"/>
+    <col min="14593" max="14593" width="8.1796875" customWidth="1"/>
     <col min="14594" max="14594" width="13" customWidth="1"/>
-    <col min="14595" max="14595" width="11.5" customWidth="1"/>
-    <col min="14596" max="14596" width="9.5" customWidth="1"/>
-    <col min="14597" max="14597" width="7.33203125" customWidth="1"/>
-    <col min="14598" max="14598" width="6.5" customWidth="1"/>
-    <col min="14599" max="14599" width="10.5" customWidth="1"/>
-    <col min="14600" max="14600" width="20.33203125" customWidth="1"/>
-    <col min="14601" max="14601" width="14.83203125" customWidth="1"/>
-    <col min="14602" max="14602" width="12.1640625" customWidth="1"/>
-    <col min="14603" max="14603" width="18.6640625" customWidth="1"/>
-    <col min="14604" max="14604" width="8.83203125" customWidth="1"/>
-    <col min="14607" max="14607" width="12.83203125" customWidth="1"/>
-    <col min="14608" max="14608" width="36.33203125" customWidth="1"/>
-    <col min="14849" max="14849" width="8.1640625" customWidth="1"/>
+    <col min="14595" max="14595" width="11.453125" customWidth="1"/>
+    <col min="14596" max="14596" width="9.453125" customWidth="1"/>
+    <col min="14597" max="14597" width="7.36328125" customWidth="1"/>
+    <col min="14598" max="14598" width="6.453125" customWidth="1"/>
+    <col min="14599" max="14599" width="10.453125" customWidth="1"/>
+    <col min="14600" max="14600" width="20.36328125" customWidth="1"/>
+    <col min="14601" max="14601" width="14.81640625" customWidth="1"/>
+    <col min="14602" max="14602" width="12.1796875" customWidth="1"/>
+    <col min="14603" max="14603" width="18.6328125" customWidth="1"/>
+    <col min="14604" max="14604" width="8.81640625" customWidth="1"/>
+    <col min="14607" max="14607" width="12.81640625" customWidth="1"/>
+    <col min="14608" max="14608" width="36.36328125" customWidth="1"/>
+    <col min="14849" max="14849" width="8.1796875" customWidth="1"/>
     <col min="14850" max="14850" width="13" customWidth="1"/>
-    <col min="14851" max="14851" width="11.5" customWidth="1"/>
-    <col min="14852" max="14852" width="9.5" customWidth="1"/>
-    <col min="14853" max="14853" width="7.33203125" customWidth="1"/>
-    <col min="14854" max="14854" width="6.5" customWidth="1"/>
-    <col min="14855" max="14855" width="10.5" customWidth="1"/>
-    <col min="14856" max="14856" width="20.33203125" customWidth="1"/>
-    <col min="14857" max="14857" width="14.83203125" customWidth="1"/>
-    <col min="14858" max="14858" width="12.1640625" customWidth="1"/>
-    <col min="14859" max="14859" width="18.6640625" customWidth="1"/>
-    <col min="14860" max="14860" width="8.83203125" customWidth="1"/>
-    <col min="14863" max="14863" width="12.83203125" customWidth="1"/>
-    <col min="14864" max="14864" width="36.33203125" customWidth="1"/>
-    <col min="15105" max="15105" width="8.1640625" customWidth="1"/>
+    <col min="14851" max="14851" width="11.453125" customWidth="1"/>
+    <col min="14852" max="14852" width="9.453125" customWidth="1"/>
+    <col min="14853" max="14853" width="7.36328125" customWidth="1"/>
+    <col min="14854" max="14854" width="6.453125" customWidth="1"/>
+    <col min="14855" max="14855" width="10.453125" customWidth="1"/>
+    <col min="14856" max="14856" width="20.36328125" customWidth="1"/>
+    <col min="14857" max="14857" width="14.81640625" customWidth="1"/>
+    <col min="14858" max="14858" width="12.1796875" customWidth="1"/>
+    <col min="14859" max="14859" width="18.6328125" customWidth="1"/>
+    <col min="14860" max="14860" width="8.81640625" customWidth="1"/>
+    <col min="14863" max="14863" width="12.81640625" customWidth="1"/>
+    <col min="14864" max="14864" width="36.36328125" customWidth="1"/>
+    <col min="15105" max="15105" width="8.1796875" customWidth="1"/>
     <col min="15106" max="15106" width="13" customWidth="1"/>
-    <col min="15107" max="15107" width="11.5" customWidth="1"/>
-    <col min="15108" max="15108" width="9.5" customWidth="1"/>
-    <col min="15109" max="15109" width="7.33203125" customWidth="1"/>
-    <col min="15110" max="15110" width="6.5" customWidth="1"/>
-    <col min="15111" max="15111" width="10.5" customWidth="1"/>
-    <col min="15112" max="15112" width="20.33203125" customWidth="1"/>
-    <col min="15113" max="15113" width="14.83203125" customWidth="1"/>
-    <col min="15114" max="15114" width="12.1640625" customWidth="1"/>
-    <col min="15115" max="15115" width="18.6640625" customWidth="1"/>
-    <col min="15116" max="15116" width="8.83203125" customWidth="1"/>
-    <col min="15119" max="15119" width="12.83203125" customWidth="1"/>
-    <col min="15120" max="15120" width="36.33203125" customWidth="1"/>
-    <col min="15361" max="15361" width="8.1640625" customWidth="1"/>
+    <col min="15107" max="15107" width="11.453125" customWidth="1"/>
+    <col min="15108" max="15108" width="9.453125" customWidth="1"/>
+    <col min="15109" max="15109" width="7.36328125" customWidth="1"/>
+    <col min="15110" max="15110" width="6.453125" customWidth="1"/>
+    <col min="15111" max="15111" width="10.453125" customWidth="1"/>
+    <col min="15112" max="15112" width="20.36328125" customWidth="1"/>
+    <col min="15113" max="15113" width="14.81640625" customWidth="1"/>
+    <col min="15114" max="15114" width="12.1796875" customWidth="1"/>
+    <col min="15115" max="15115" width="18.6328125" customWidth="1"/>
+    <col min="15116" max="15116" width="8.81640625" customWidth="1"/>
+    <col min="15119" max="15119" width="12.81640625" customWidth="1"/>
+    <col min="15120" max="15120" width="36.36328125" customWidth="1"/>
+    <col min="15361" max="15361" width="8.1796875" customWidth="1"/>
     <col min="15362" max="15362" width="13" customWidth="1"/>
-    <col min="15363" max="15363" width="11.5" customWidth="1"/>
-    <col min="15364" max="15364" width="9.5" customWidth="1"/>
-    <col min="15365" max="15365" width="7.33203125" customWidth="1"/>
-    <col min="15366" max="15366" width="6.5" customWidth="1"/>
-    <col min="15367" max="15367" width="10.5" customWidth="1"/>
-    <col min="15368" max="15368" width="20.33203125" customWidth="1"/>
-    <col min="15369" max="15369" width="14.83203125" customWidth="1"/>
-    <col min="15370" max="15370" width="12.1640625" customWidth="1"/>
-    <col min="15371" max="15371" width="18.6640625" customWidth="1"/>
-    <col min="15372" max="15372" width="8.83203125" customWidth="1"/>
-    <col min="15375" max="15375" width="12.83203125" customWidth="1"/>
-    <col min="15376" max="15376" width="36.33203125" customWidth="1"/>
-    <col min="15617" max="15617" width="8.1640625" customWidth="1"/>
+    <col min="15363" max="15363" width="11.453125" customWidth="1"/>
+    <col min="15364" max="15364" width="9.453125" customWidth="1"/>
+    <col min="15365" max="15365" width="7.36328125" customWidth="1"/>
+    <col min="15366" max="15366" width="6.453125" customWidth="1"/>
+    <col min="15367" max="15367" width="10.453125" customWidth="1"/>
+    <col min="15368" max="15368" width="20.36328125" customWidth="1"/>
+    <col min="15369" max="15369" width="14.81640625" customWidth="1"/>
+    <col min="15370" max="15370" width="12.1796875" customWidth="1"/>
+    <col min="15371" max="15371" width="18.6328125" customWidth="1"/>
+    <col min="15372" max="15372" width="8.81640625" customWidth="1"/>
+    <col min="15375" max="15375" width="12.81640625" customWidth="1"/>
+    <col min="15376" max="15376" width="36.36328125" customWidth="1"/>
+    <col min="15617" max="15617" width="8.1796875" customWidth="1"/>
     <col min="15618" max="15618" width="13" customWidth="1"/>
-    <col min="15619" max="15619" width="11.5" customWidth="1"/>
-    <col min="15620" max="15620" width="9.5" customWidth="1"/>
-    <col min="15621" max="15621" width="7.33203125" customWidth="1"/>
-    <col min="15622" max="15622" width="6.5" customWidth="1"/>
-    <col min="15623" max="15623" width="10.5" customWidth="1"/>
-    <col min="15624" max="15624" width="20.33203125" customWidth="1"/>
-    <col min="15625" max="15625" width="14.83203125" customWidth="1"/>
-    <col min="15626" max="15626" width="12.1640625" customWidth="1"/>
-    <col min="15627" max="15627" width="18.6640625" customWidth="1"/>
-    <col min="15628" max="15628" width="8.83203125" customWidth="1"/>
-    <col min="15631" max="15631" width="12.83203125" customWidth="1"/>
-    <col min="15632" max="15632" width="36.33203125" customWidth="1"/>
-    <col min="15873" max="15873" width="8.1640625" customWidth="1"/>
+    <col min="15619" max="15619" width="11.453125" customWidth="1"/>
+    <col min="15620" max="15620" width="9.453125" customWidth="1"/>
+    <col min="15621" max="15621" width="7.36328125" customWidth="1"/>
+    <col min="15622" max="15622" width="6.453125" customWidth="1"/>
+    <col min="15623" max="15623" width="10.453125" customWidth="1"/>
+    <col min="15624" max="15624" width="20.36328125" customWidth="1"/>
+    <col min="15625" max="15625" width="14.81640625" customWidth="1"/>
+    <col min="15626" max="15626" width="12.1796875" customWidth="1"/>
+    <col min="15627" max="15627" width="18.6328125" customWidth="1"/>
+    <col min="15628" max="15628" width="8.81640625" customWidth="1"/>
+    <col min="15631" max="15631" width="12.81640625" customWidth="1"/>
+    <col min="15632" max="15632" width="36.36328125" customWidth="1"/>
+    <col min="15873" max="15873" width="8.1796875" customWidth="1"/>
     <col min="15874" max="15874" width="13" customWidth="1"/>
-    <col min="15875" max="15875" width="11.5" customWidth="1"/>
-    <col min="15876" max="15876" width="9.5" customWidth="1"/>
-    <col min="15877" max="15877" width="7.33203125" customWidth="1"/>
-    <col min="15878" max="15878" width="6.5" customWidth="1"/>
-    <col min="15879" max="15879" width="10.5" customWidth="1"/>
-    <col min="15880" max="15880" width="20.33203125" customWidth="1"/>
-    <col min="15881" max="15881" width="14.83203125" customWidth="1"/>
-    <col min="15882" max="15882" width="12.1640625" customWidth="1"/>
-    <col min="15883" max="15883" width="18.6640625" customWidth="1"/>
-    <col min="15884" max="15884" width="8.83203125" customWidth="1"/>
-    <col min="15887" max="15887" width="12.83203125" customWidth="1"/>
-    <col min="15888" max="15888" width="36.33203125" customWidth="1"/>
-    <col min="16129" max="16129" width="8.1640625" customWidth="1"/>
+    <col min="15875" max="15875" width="11.453125" customWidth="1"/>
+    <col min="15876" max="15876" width="9.453125" customWidth="1"/>
+    <col min="15877" max="15877" width="7.36328125" customWidth="1"/>
+    <col min="15878" max="15878" width="6.453125" customWidth="1"/>
+    <col min="15879" max="15879" width="10.453125" customWidth="1"/>
+    <col min="15880" max="15880" width="20.36328125" customWidth="1"/>
+    <col min="15881" max="15881" width="14.81640625" customWidth="1"/>
+    <col min="15882" max="15882" width="12.1796875" customWidth="1"/>
+    <col min="15883" max="15883" width="18.6328125" customWidth="1"/>
+    <col min="15884" max="15884" width="8.81640625" customWidth="1"/>
+    <col min="15887" max="15887" width="12.81640625" customWidth="1"/>
+    <col min="15888" max="15888" width="36.36328125" customWidth="1"/>
+    <col min="16129" max="16129" width="8.1796875" customWidth="1"/>
     <col min="16130" max="16130" width="13" customWidth="1"/>
-    <col min="16131" max="16131" width="11.5" customWidth="1"/>
-    <col min="16132" max="16132" width="9.5" customWidth="1"/>
-    <col min="16133" max="16133" width="7.33203125" customWidth="1"/>
-    <col min="16134" max="16134" width="6.5" customWidth="1"/>
-    <col min="16135" max="16135" width="10.5" customWidth="1"/>
-    <col min="16136" max="16136" width="20.33203125" customWidth="1"/>
-    <col min="16137" max="16137" width="14.83203125" customWidth="1"/>
-    <col min="16138" max="16138" width="12.1640625" customWidth="1"/>
-    <col min="16139" max="16139" width="18.6640625" customWidth="1"/>
-    <col min="16140" max="16140" width="8.83203125" customWidth="1"/>
-    <col min="16143" max="16143" width="12.83203125" customWidth="1"/>
-    <col min="16144" max="16144" width="36.33203125" customWidth="1"/>
+    <col min="16131" max="16131" width="11.453125" customWidth="1"/>
+    <col min="16132" max="16132" width="9.453125" customWidth="1"/>
+    <col min="16133" max="16133" width="7.36328125" customWidth="1"/>
+    <col min="16134" max="16134" width="6.453125" customWidth="1"/>
+    <col min="16135" max="16135" width="10.453125" customWidth="1"/>
+    <col min="16136" max="16136" width="20.36328125" customWidth="1"/>
+    <col min="16137" max="16137" width="14.81640625" customWidth="1"/>
+    <col min="16138" max="16138" width="12.1796875" customWidth="1"/>
+    <col min="16139" max="16139" width="18.6328125" customWidth="1"/>
+    <col min="16140" max="16140" width="8.81640625" customWidth="1"/>
+    <col min="16143" max="16143" width="12.81640625" customWidth="1"/>
+    <col min="16144" max="16144" width="36.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>368</v>
       </c>
@@ -3394,7 +3416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1">
+    <row r="2" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>369</v>
       </c>
@@ -3444,7 +3466,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="12" customFormat="1">
+    <row r="3" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3498,7 +3520,7 @@
       <c r="R3"/>
       <c r="S3"/>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1">
+    <row r="4" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>374</v>
       </c>
@@ -3551,7 +3573,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1">
+    <row r="5" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>56</v>
       </c>
@@ -3605,7 +3627,7 @@
       <c r="R5"/>
       <c r="S5"/>
     </row>
-    <row r="6" spans="1:19" s="12" customFormat="1">
+    <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>57</v>
       </c>
@@ -3659,7 +3681,7 @@
       <c r="R6"/>
       <c r="S6"/>
     </row>
-    <row r="7" spans="1:19" s="12" customFormat="1">
+    <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>375</v>
       </c>
@@ -3712,7 +3734,7 @@
       <c r="R7"/>
       <c r="S7"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>60</v>
       </c>
@@ -3763,7 +3785,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>61</v>
       </c>
@@ -3814,7 +3836,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>377</v>
       </c>
@@ -3864,7 +3886,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
@@ -3915,7 +3937,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>64</v>
       </c>
@@ -3965,7 +3987,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>379</v>
       </c>
@@ -4015,7 +4037,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>70</v>
       </c>
@@ -4066,7 +4088,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>71</v>
       </c>
@@ -4116,7 +4138,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>73</v>
       </c>
@@ -4167,7 +4189,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>75</v>
       </c>
@@ -4218,7 +4240,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>76</v>
       </c>
@@ -4269,7 +4291,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="28">
+    <row r="19" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>77</v>
       </c>
@@ -4320,7 +4342,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>376</v>
       </c>
@@ -4370,7 +4392,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="28">
+    <row r="21" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>81</v>
       </c>
@@ -4420,7 +4442,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>85</v>
       </c>
@@ -4470,7 +4492,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>380</v>
       </c>
@@ -4520,7 +4542,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>88</v>
       </c>
@@ -4571,7 +4593,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>90</v>
       </c>
@@ -4622,7 +4644,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>92</v>
       </c>
@@ -4673,7 +4695,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>381</v>
       </c>
@@ -4723,7 +4745,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>93</v>
       </c>
@@ -4774,7 +4796,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>382</v>
       </c>
@@ -4824,7 +4846,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>94</v>
       </c>
@@ -4875,7 +4897,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>383</v>
       </c>
@@ -4925,7 +4947,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>97</v>
       </c>
@@ -4975,7 +4997,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>384</v>
       </c>
@@ -5025,7 +5047,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
         <v>101</v>
       </c>
@@ -5075,7 +5097,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
         <v>385</v>
       </c>
@@ -5125,7 +5147,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
         <v>386</v>
       </c>
@@ -5175,7 +5197,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
         <v>387</v>
       </c>
@@ -5225,7 +5247,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
         <v>388</v>
       </c>
@@ -5275,7 +5297,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
         <v>102</v>
       </c>
@@ -5326,7 +5348,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>104</v>
       </c>
@@ -5377,7 +5399,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
         <v>105</v>
       </c>
@@ -5428,7 +5450,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="42">
+    <row r="42" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
         <v>402</v>
       </c>
@@ -5478,7 +5500,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>106</v>
       </c>
@@ -5529,7 +5551,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
         <v>108</v>
       </c>
@@ -5581,7 +5603,7 @@
       </c>
       <c r="S44" s="3"/>
     </row>
-    <row r="45" spans="1:19" ht="28">
+    <row r="45" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
         <v>109</v>
       </c>
@@ -5633,7 +5655,7 @@
       </c>
       <c r="S45" s="3"/>
     </row>
-    <row r="46" spans="1:19" ht="42">
+    <row r="46" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
         <v>403</v>
       </c>
@@ -5683,7 +5705,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>111</v>
       </c>
@@ -5734,7 +5756,7 @@
       </c>
       <c r="S47" s="3"/>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>113</v>
       </c>
@@ -5786,7 +5808,7 @@
       </c>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
         <v>117</v>
       </c>
@@ -5838,7 +5860,7 @@
       </c>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
         <v>118</v>
       </c>
@@ -5890,7 +5912,7 @@
       </c>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
         <v>119</v>
       </c>
@@ -5941,7 +5963,7 @@
       </c>
       <c r="S51" s="3"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
         <v>121</v>
       </c>
@@ -5993,7 +6015,7 @@
       </c>
       <c r="S52" s="3"/>
     </row>
-    <row r="53" spans="1:19" ht="28">
+    <row r="53" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
         <v>122</v>
       </c>
@@ -6044,7 +6066,7 @@
       </c>
       <c r="S53" s="3"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
         <v>124</v>
       </c>
@@ -6095,7 +6117,7 @@
       </c>
       <c r="S54" s="3"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
         <v>126</v>
       </c>
@@ -6147,7 +6169,7 @@
       </c>
       <c r="S55" s="3"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
         <v>127</v>
       </c>
@@ -6199,7 +6221,7 @@
       </c>
       <c r="S56" s="3"/>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
         <v>128</v>
       </c>
@@ -6251,7 +6273,7 @@
       </c>
       <c r="S57" s="3"/>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
         <v>129</v>
       </c>
@@ -6303,7 +6325,7 @@
       </c>
       <c r="S58" s="3"/>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
         <v>130</v>
       </c>
@@ -6355,7 +6377,7 @@
       </c>
       <c r="S59" s="3"/>
     </row>
-    <row r="60" spans="1:19" ht="42">
+    <row r="60" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
         <v>404</v>
       </c>
@@ -6405,7 +6427,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
         <v>133</v>
       </c>
@@ -6457,7 +6479,7 @@
       </c>
       <c r="S61" s="3"/>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="15" t="s">
         <v>135</v>
       </c>
@@ -6509,7 +6531,7 @@
       </c>
       <c r="S62" s="3"/>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
         <v>137</v>
       </c>
@@ -6561,7 +6583,7 @@
       </c>
       <c r="S63" s="3"/>
     </row>
-    <row r="64" spans="1:19" ht="13.5" customHeight="1">
+    <row r="64" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="15" t="s">
         <v>138</v>
       </c>
@@ -6613,7 +6635,7 @@
       </c>
       <c r="S64" s="3"/>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="15" t="s">
         <v>139</v>
       </c>
@@ -6665,7 +6687,7 @@
       </c>
       <c r="S65" s="3"/>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="15" t="s">
         <v>140</v>
       </c>
@@ -6717,7 +6739,7 @@
       </c>
       <c r="S66" s="3"/>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="15" t="s">
         <v>141</v>
       </c>
@@ -6769,7 +6791,7 @@
       </c>
       <c r="S67" s="3"/>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="15" t="s">
         <v>142</v>
       </c>
@@ -6821,7 +6843,7 @@
       </c>
       <c r="S68" s="3"/>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="15" t="s">
         <v>144</v>
       </c>
@@ -6873,7 +6895,7 @@
       </c>
       <c r="S69" s="3"/>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>145</v>
       </c>
@@ -6924,7 +6946,7 @@
       </c>
       <c r="S70" s="3"/>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>147</v>
       </c>
@@ -6976,7 +6998,7 @@
       </c>
       <c r="S71" s="3"/>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="15" t="s">
         <v>148</v>
       </c>
@@ -7028,7 +7050,7 @@
       </c>
       <c r="S72" s="3"/>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
         <v>150</v>
       </c>
@@ -7080,7 +7102,7 @@
       </c>
       <c r="S73" s="3"/>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="15" t="s">
         <v>151</v>
       </c>
@@ -7132,7 +7154,7 @@
       </c>
       <c r="S74" s="3"/>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" s="15" t="s">
         <v>152</v>
       </c>
@@ -7184,7 +7206,7 @@
       </c>
       <c r="S75" s="3"/>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="15" t="s">
         <v>153</v>
       </c>
@@ -7236,7 +7258,7 @@
       </c>
       <c r="S76" s="3"/>
     </row>
-    <row r="77" spans="1:19" ht="28">
+    <row r="77" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="15" t="s">
         <v>154</v>
       </c>
@@ -7288,7 +7310,7 @@
       </c>
       <c r="S77" s="3"/>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
         <v>156</v>
       </c>
@@ -7340,7 +7362,7 @@
       </c>
       <c r="S78" s="3"/>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
         <v>158</v>
       </c>
@@ -7392,7 +7414,7 @@
       </c>
       <c r="S79" s="3"/>
     </row>
-    <row r="80" spans="1:19" ht="28">
+    <row r="80" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="15" t="s">
         <v>159</v>
       </c>
@@ -7444,7 +7466,7 @@
       </c>
       <c r="S80" s="3"/>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="15" t="s">
         <v>162</v>
       </c>
@@ -7496,7 +7518,7 @@
       </c>
       <c r="S81" s="3"/>
     </row>
-    <row r="82" spans="1:19" ht="26.25" customHeight="1">
+    <row r="82" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="15" t="s">
         <v>163</v>
       </c>
@@ -7548,7 +7570,7 @@
       </c>
       <c r="S82" s="3"/>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" s="15" t="s">
         <v>164</v>
       </c>
@@ -7600,7 +7622,7 @@
       </c>
       <c r="S83" s="3"/>
     </row>
-    <row r="84" spans="1:19">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
         <v>167</v>
       </c>
@@ -7652,7 +7674,7 @@
       </c>
       <c r="S84" s="3"/>
     </row>
-    <row r="85" spans="1:19" ht="28">
+    <row r="85" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="15" t="s">
         <v>168</v>
       </c>
@@ -7703,7 +7725,7 @@
       </c>
       <c r="S85" s="3"/>
     </row>
-    <row r="86" spans="1:19" ht="28">
+    <row r="86" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="15" t="s">
         <v>171</v>
       </c>
@@ -7755,7 +7777,7 @@
       </c>
       <c r="S86" s="3"/>
     </row>
-    <row r="87" spans="1:19" ht="28">
+    <row r="87" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
         <v>174</v>
       </c>
@@ -7807,7 +7829,7 @@
       </c>
       <c r="S87" s="3"/>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" s="15" t="s">
         <v>175</v>
       </c>
@@ -7858,7 +7880,7 @@
       </c>
       <c r="S88" s="3"/>
     </row>
-    <row r="89" spans="1:19" ht="26.25" customHeight="1">
+    <row r="89" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="15" t="s">
         <v>176</v>
       </c>
@@ -7909,7 +7931,7 @@
       </c>
       <c r="S89" s="3"/>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
         <v>181</v>
       </c>
@@ -7961,7 +7983,7 @@
       </c>
       <c r="S90" s="3"/>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A91" s="15" t="s">
         <v>182</v>
       </c>
@@ -8013,7 +8035,7 @@
       </c>
       <c r="S91" s="3"/>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" s="15" t="s">
         <v>183</v>
       </c>
@@ -8065,7 +8087,7 @@
       </c>
       <c r="S92" s="3"/>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" s="15" t="s">
         <v>184</v>
       </c>
@@ -8117,7 +8139,7 @@
       </c>
       <c r="S93" s="3"/>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" s="15" t="s">
         <v>185</v>
       </c>
@@ -8169,7 +8191,7 @@
       </c>
       <c r="S94" s="3"/>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" s="15" t="s">
         <v>186</v>
       </c>
@@ -8221,7 +8243,7 @@
       </c>
       <c r="S95" s="3"/>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
         <v>187</v>
       </c>
@@ -8272,7 +8294,7 @@
       </c>
       <c r="S96" s="3"/>
     </row>
-    <row r="97" spans="1:19">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" s="15" t="s">
         <v>188</v>
       </c>
@@ -8323,7 +8345,7 @@
       </c>
       <c r="S97" s="3"/>
     </row>
-    <row r="98" spans="1:19">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="15" t="s">
         <v>189</v>
       </c>
@@ -8374,7 +8396,7 @@
       </c>
       <c r="S98" s="3"/>
     </row>
-    <row r="99" spans="1:19">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" s="15" t="s">
         <v>190</v>
       </c>
@@ -8425,7 +8447,7 @@
       </c>
       <c r="S99" s="3"/>
     </row>
-    <row r="100" spans="1:19">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" s="15" t="s">
         <v>191</v>
       </c>
@@ -8477,7 +8499,7 @@
       </c>
       <c r="S100" s="3"/>
     </row>
-    <row r="101" spans="1:19">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" s="15" t="s">
         <v>192</v>
       </c>
@@ -8529,7 +8551,7 @@
       </c>
       <c r="S101" s="3"/>
     </row>
-    <row r="102" spans="1:19">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
         <v>193</v>
       </c>
@@ -8581,7 +8603,7 @@
       </c>
       <c r="S102" s="3"/>
     </row>
-    <row r="103" spans="1:19">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="15" t="s">
         <v>194</v>
       </c>
@@ -8633,7 +8655,7 @@
       </c>
       <c r="S103" s="3"/>
     </row>
-    <row r="104" spans="1:19">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" s="15" t="s">
         <v>195</v>
       </c>
@@ -8685,7 +8707,7 @@
       </c>
       <c r="S104" s="3"/>
     </row>
-    <row r="105" spans="1:19">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" s="15" t="s">
         <v>196</v>
       </c>
@@ -8737,7 +8759,7 @@
       </c>
       <c r="S105" s="3"/>
     </row>
-    <row r="106" spans="1:19">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" s="15" t="s">
         <v>197</v>
       </c>
@@ -8789,7 +8811,7 @@
       </c>
       <c r="S106" s="3"/>
     </row>
-    <row r="107" spans="1:19">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" s="15" t="s">
         <v>199</v>
       </c>
@@ -8841,7 +8863,7 @@
       </c>
       <c r="S107" s="3"/>
     </row>
-    <row r="108" spans="1:19">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
         <v>200</v>
       </c>
@@ -8893,7 +8915,7 @@
       </c>
       <c r="S108" s="3"/>
     </row>
-    <row r="109" spans="1:19">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" s="15" t="s">
         <v>201</v>
       </c>
@@ -8945,7 +8967,7 @@
       </c>
       <c r="S109" s="3"/>
     </row>
-    <row r="110" spans="1:19">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="15" t="s">
         <v>202</v>
       </c>
@@ -8997,7 +9019,7 @@
       </c>
       <c r="S110" s="3"/>
     </row>
-    <row r="111" spans="1:19">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" s="15" t="s">
         <v>203</v>
       </c>
@@ -9049,7 +9071,7 @@
       </c>
       <c r="S111" s="3"/>
     </row>
-    <row r="112" spans="1:19">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" s="15" t="s">
         <v>204</v>
       </c>
@@ -9101,7 +9123,7 @@
       </c>
       <c r="S112" s="3"/>
     </row>
-    <row r="113" spans="1:19">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" s="15" t="s">
         <v>205</v>
       </c>
@@ -9153,7 +9175,7 @@
       </c>
       <c r="S113" s="3"/>
     </row>
-    <row r="114" spans="1:19">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" s="15" t="s">
         <v>206</v>
       </c>
@@ -9205,7 +9227,7 @@
       </c>
       <c r="S114" s="3"/>
     </row>
-    <row r="115" spans="1:19">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
         <v>206</v>
       </c>
@@ -9256,7 +9278,7 @@
       </c>
       <c r="S115" s="3"/>
     </row>
-    <row r="116" spans="1:19">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" s="15" t="s">
         <v>208</v>
       </c>
@@ -9308,7 +9330,7 @@
       </c>
       <c r="S116" s="3"/>
     </row>
-    <row r="117" spans="1:19">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" s="15" t="s">
         <v>209</v>
       </c>
@@ -9360,7 +9382,7 @@
       </c>
       <c r="S117" s="3"/>
     </row>
-    <row r="118" spans="1:19">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" s="15" t="s">
         <v>211</v>
       </c>
@@ -9412,7 +9434,7 @@
       </c>
       <c r="S118" s="3"/>
     </row>
-    <row r="119" spans="1:19">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" s="15" t="s">
         <v>212</v>
       </c>
@@ -9464,7 +9486,7 @@
       </c>
       <c r="S119" s="3"/>
     </row>
-    <row r="120" spans="1:19">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" s="15" t="s">
         <v>213</v>
       </c>
@@ -9516,7 +9538,7 @@
       </c>
       <c r="S120" s="3"/>
     </row>
-    <row r="121" spans="1:19">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" s="15" t="s">
         <v>215</v>
       </c>
@@ -9568,7 +9590,7 @@
       </c>
       <c r="S121" s="3"/>
     </row>
-    <row r="122" spans="1:19">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
         <v>216</v>
       </c>
@@ -9620,7 +9642,7 @@
       </c>
       <c r="S122" s="3"/>
     </row>
-    <row r="123" spans="1:19" ht="13.5" customHeight="1">
+    <row r="123" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="15" t="s">
         <v>217</v>
       </c>
@@ -9671,7 +9693,7 @@
       </c>
       <c r="S123" s="3"/>
     </row>
-    <row r="124" spans="1:19" ht="16.5" customHeight="1">
+    <row r="124" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="15" t="s">
         <v>218</v>
       </c>
@@ -9723,7 +9745,7 @@
       </c>
       <c r="S124" s="3"/>
     </row>
-    <row r="125" spans="1:19">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" s="15" t="s">
         <v>219</v>
       </c>
@@ -9774,7 +9796,7 @@
       </c>
       <c r="S125" s="3"/>
     </row>
-    <row r="126" spans="1:19" ht="42">
+    <row r="126" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A126" s="15" t="s">
         <v>220</v>
       </c>
@@ -9825,7 +9847,7 @@
       </c>
       <c r="S126" s="3"/>
     </row>
-    <row r="127" spans="1:19" ht="42">
+    <row r="127" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A127" s="15" t="s">
         <v>221</v>
       </c>
@@ -9876,7 +9898,7 @@
       </c>
       <c r="S127" s="3"/>
     </row>
-    <row r="128" spans="1:19" ht="42">
+    <row r="128" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="15" t="s">
         <v>222</v>
       </c>
@@ -9927,7 +9949,7 @@
       </c>
       <c r="S128" s="3"/>
     </row>
-    <row r="129" spans="1:19" ht="42">
+    <row r="129" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
         <v>223</v>
       </c>
@@ -9978,7 +10000,7 @@
       </c>
       <c r="S129" s="3"/>
     </row>
-    <row r="130" spans="1:19" ht="28">
+    <row r="130" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="15" t="s">
         <v>224</v>
       </c>
@@ -10029,7 +10051,7 @@
       </c>
       <c r="S130" s="3"/>
     </row>
-    <row r="131" spans="1:19">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="15" t="s">
         <v>226</v>
       </c>
@@ -10081,7 +10103,7 @@
       </c>
       <c r="S131" s="3"/>
     </row>
-    <row r="132" spans="1:19" ht="15" customHeight="1">
+    <row r="132" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="15" t="s">
         <v>227</v>
       </c>
@@ -10133,7 +10155,7 @@
       </c>
       <c r="S132" s="3"/>
     </row>
-    <row r="133" spans="1:19" ht="15" customHeight="1">
+    <row r="133" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="15" t="s">
         <v>228</v>
       </c>
@@ -10184,7 +10206,7 @@
       </c>
       <c r="S133" s="3"/>
     </row>
-    <row r="134" spans="1:19" ht="18" customHeight="1">
+    <row r="134" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="15" t="s">
         <v>231</v>
       </c>
@@ -10236,7 +10258,7 @@
       </c>
       <c r="S134" s="3"/>
     </row>
-    <row r="135" spans="1:19" ht="14.25" customHeight="1">
+    <row r="135" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="15" t="s">
         <v>233</v>
       </c>
@@ -10287,7 +10309,7 @@
       </c>
       <c r="S135" s="3"/>
     </row>
-    <row r="136" spans="1:19">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="15" t="s">
         <v>235</v>
       </c>
@@ -10338,7 +10360,7 @@
       </c>
       <c r="S136" s="3"/>
     </row>
-    <row r="137" spans="1:19">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" s="15" t="s">
         <v>236</v>
       </c>
@@ -10390,7 +10412,7 @@
       </c>
       <c r="S137" s="3"/>
     </row>
-    <row r="138" spans="1:19" ht="37.5" customHeight="1">
+    <row r="138" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
         <v>237</v>
       </c>
@@ -10441,7 +10463,7 @@
       </c>
       <c r="S138" s="3"/>
     </row>
-    <row r="139" spans="1:19" ht="39.75" customHeight="1">
+    <row r="139" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
         <v>238</v>
       </c>
@@ -10492,7 +10514,7 @@
       </c>
       <c r="S139" s="3"/>
     </row>
-    <row r="140" spans="1:19" ht="48" customHeight="1">
+    <row r="140" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
         <v>241</v>
       </c>
@@ -10543,7 +10565,7 @@
       </c>
       <c r="S140" s="3"/>
     </row>
-    <row r="141" spans="1:19">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="15" t="s">
         <v>242</v>
       </c>
@@ -10595,7 +10617,7 @@
       </c>
       <c r="S141" s="3"/>
     </row>
-    <row r="142" spans="1:19">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="15" t="s">
         <v>242</v>
       </c>
@@ -10646,7 +10668,7 @@
       </c>
       <c r="S142" s="3"/>
     </row>
-    <row r="143" spans="1:19">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" s="15" t="s">
         <v>243</v>
       </c>
@@ -10698,7 +10720,7 @@
       </c>
       <c r="S143" s="3"/>
     </row>
-    <row r="144" spans="1:19">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="15" t="s">
         <v>244</v>
       </c>
@@ -10750,7 +10772,7 @@
       </c>
       <c r="S144" s="3"/>
     </row>
-    <row r="145" spans="1:19">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" s="15" t="s">
         <v>245</v>
       </c>
@@ -10802,7 +10824,7 @@
       </c>
       <c r="S145" s="3"/>
     </row>
-    <row r="146" spans="1:19">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" s="15" t="s">
         <v>247</v>
       </c>
@@ -10854,7 +10876,7 @@
       </c>
       <c r="S146" s="3"/>
     </row>
-    <row r="147" spans="1:19">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" s="15" t="s">
         <v>248</v>
       </c>
@@ -10906,7 +10928,7 @@
       </c>
       <c r="S147" s="3"/>
     </row>
-    <row r="148" spans="1:19">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" s="15" t="s">
         <v>250</v>
       </c>
@@ -10958,7 +10980,7 @@
       </c>
       <c r="S148" s="3"/>
     </row>
-    <row r="149" spans="1:19">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A149" s="15" t="s">
         <v>251</v>
       </c>
@@ -11010,7 +11032,7 @@
       </c>
       <c r="S149" s="3"/>
     </row>
-    <row r="150" spans="1:19">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A150" s="15" t="s">
         <v>252</v>
       </c>
@@ -11062,7 +11084,7 @@
       </c>
       <c r="S150" s="3"/>
     </row>
-    <row r="151" spans="1:19">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A151" s="15" t="s">
         <v>253</v>
       </c>
@@ -11114,7 +11136,7 @@
       </c>
       <c r="S151" s="3"/>
     </row>
-    <row r="152" spans="1:19">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A152" s="15" t="s">
         <v>254</v>
       </c>
@@ -11166,7 +11188,7 @@
       </c>
       <c r="S152" s="3"/>
     </row>
-    <row r="153" spans="1:19">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" s="15" t="s">
         <v>256</v>
       </c>
@@ -11217,7 +11239,7 @@
       </c>
       <c r="S153" s="3"/>
     </row>
-    <row r="154" spans="1:19" ht="3.75" customHeight="1">
+    <row r="154" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="15" t="s">
         <v>257</v>
       </c>
@@ -11269,7 +11291,7 @@
       </c>
       <c r="S154" s="3"/>
     </row>
-    <row r="155" spans="1:19">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" s="15" t="s">
         <v>258</v>
       </c>
@@ -11321,7 +11343,7 @@
       </c>
       <c r="S155" s="3"/>
     </row>
-    <row r="156" spans="1:19">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A156" s="15" t="s">
         <v>260</v>
       </c>
@@ -11373,7 +11395,7 @@
       </c>
       <c r="S156" s="3"/>
     </row>
-    <row r="157" spans="1:19">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A157" s="15" t="s">
         <v>261</v>
       </c>
@@ -11425,7 +11447,7 @@
       </c>
       <c r="S157" s="3"/>
     </row>
-    <row r="158" spans="1:19">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A158" s="15" t="s">
         <v>262</v>
       </c>
@@ -11477,7 +11499,7 @@
       </c>
       <c r="S158" s="3"/>
     </row>
-    <row r="159" spans="1:19">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A159" s="15" t="s">
         <v>263</v>
       </c>
@@ -11529,7 +11551,7 @@
       </c>
       <c r="S159" s="3"/>
     </row>
-    <row r="160" spans="1:19">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A160" s="15" t="s">
         <v>264</v>
       </c>
@@ -11581,7 +11603,7 @@
       </c>
       <c r="S160" s="3"/>
     </row>
-    <row r="161" spans="1:19">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A161" s="15" t="s">
         <v>415</v>
       </c>
@@ -11631,7 +11653,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="162" spans="1:19">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A162" s="15" t="s">
         <v>417</v>
       </c>
@@ -11681,7 +11703,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="24" customHeight="1">
+    <row r="163" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="15" t="s">
         <v>265</v>
       </c>
@@ -11733,7 +11755,7 @@
       </c>
       <c r="S163" s="3"/>
     </row>
-    <row r="164" spans="1:19" ht="24" customHeight="1">
+    <row r="164" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="15" t="s">
         <v>267</v>
       </c>
@@ -11785,7 +11807,7 @@
       </c>
       <c r="S164" s="3"/>
     </row>
-    <row r="165" spans="1:19" ht="24" customHeight="1">
+    <row r="165" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="15" t="s">
         <v>269</v>
       </c>
@@ -11837,7 +11859,7 @@
       </c>
       <c r="S165" s="3"/>
     </row>
-    <row r="166" spans="1:19">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A166" s="15" t="s">
         <v>270</v>
       </c>
@@ -11889,7 +11911,7 @@
       </c>
       <c r="S166" s="3"/>
     </row>
-    <row r="167" spans="1:19">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A167" s="15" t="s">
         <v>271</v>
       </c>
@@ -11940,7 +11962,7 @@
       </c>
       <c r="S167" s="3"/>
     </row>
-    <row r="168" spans="1:19" ht="28">
+    <row r="168" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A168" s="15" t="s">
         <v>272</v>
       </c>
@@ -11991,7 +12013,7 @@
       </c>
       <c r="S168" s="3"/>
     </row>
-    <row r="169" spans="1:19" ht="28">
+    <row r="169" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="15" t="s">
         <v>274</v>
       </c>
@@ -12042,7 +12064,7 @@
       </c>
       <c r="S169" s="3"/>
     </row>
-    <row r="170" spans="1:19" ht="28">
+    <row r="170" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="15" t="s">
         <v>275</v>
       </c>
@@ -12093,58 +12115,58 @@
       </c>
       <c r="S170" s="3"/>
     </row>
-    <row r="171" spans="1:19" ht="28">
-      <c r="A171" s="15" t="s">
+    <row r="171" spans="1:19" s="19" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A171" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D171" t="s">
-        <v>49</v>
-      </c>
-      <c r="E171" t="s">
+      <c r="D171" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E171" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F171" t="s">
-        <v>51</v>
-      </c>
-      <c r="G171" s="3">
+      <c r="F171" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G171" s="20">
         <v>12</v>
       </c>
-      <c r="H171" s="9" t="s">
+      <c r="H171" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="I171" s="9" t="s">
+      <c r="I171" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="J171" s="9" t="s">
+      <c r="J171" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="K171" s="10" t="s">
+      <c r="K171" s="22" t="s">
         <v>439</v>
       </c>
-      <c r="L171" s="9" t="s">
+      <c r="L171" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="M171" s="3" t="s">
+      <c r="M171" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="N171" s="3" t="s">
+      <c r="N171" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="O171" s="3" t="s">
+      <c r="O171" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="P171" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="S171" s="3"/>
-    </row>
-    <row r="172" spans="1:19">
+      <c r="P171" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="S171" s="20"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A172" s="15" t="s">
         <v>277</v>
       </c>
@@ -12196,7 +12218,7 @@
       </c>
       <c r="S172" s="3"/>
     </row>
-    <row r="173" spans="1:19" ht="42">
+    <row r="173" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A173" s="15" t="s">
         <v>414</v>
       </c>
@@ -12248,7 +12270,7 @@
       </c>
       <c r="S173" s="3"/>
     </row>
-    <row r="174" spans="1:19">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A174" s="15" t="s">
         <v>278</v>
       </c>
@@ -12298,7 +12320,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="175" spans="1:19">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A175" s="15" t="s">
         <v>279</v>
       </c>
@@ -12349,7 +12371,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="28">
+    <row r="176" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="15" t="s">
         <v>280</v>
       </c>
@@ -12400,7 +12422,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A177" s="15" t="s">
         <v>281</v>
       </c>
@@ -12451,7 +12473,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A178" s="15" t="s">
         <v>282</v>
       </c>
@@ -12502,7 +12524,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A179" s="15" t="s">
         <v>283</v>
       </c>
@@ -12552,7 +12574,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="28">
+    <row r="180" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="15" t="s">
         <v>284</v>
       </c>
@@ -12602,7 +12624,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="28">
+    <row r="181" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="15" t="s">
         <v>285</v>
       </c>
@@ -12652,7 +12674,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="28">
+    <row r="182" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="15" t="s">
         <v>286</v>
       </c>
@@ -12702,7 +12724,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="28">
+    <row r="183" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="15" t="s">
         <v>287</v>
       </c>
@@ -12752,7 +12774,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A184" s="15" t="s">
         <v>288</v>
       </c>
@@ -12803,7 +12825,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="42">
+    <row r="185" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A185" s="15" t="s">
         <v>413</v>
       </c>
@@ -12854,7 +12876,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A186" s="15" t="s">
         <v>289</v>
       </c>
@@ -12905,7 +12927,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A187" s="15" t="s">
         <v>290</v>
       </c>
@@ -12955,7 +12977,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="42">
+    <row r="188" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A188" s="15" t="s">
         <v>291</v>
       </c>
@@ -13005,7 +13027,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="189" spans="1:16" ht="28">
+    <row r="189" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A189" s="15" t="s">
         <v>292</v>
       </c>
@@ -13055,7 +13077,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="190" spans="1:16" ht="28">
+    <row r="190" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
         <v>293</v>
       </c>
@@ -13105,7 +13127,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="191" spans="1:16" ht="28">
+    <row r="191" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="15" t="s">
         <v>294</v>
       </c>
@@ -13156,7 +13178,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="192" spans="1:16" ht="15" customHeight="1">
+    <row r="192" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="15" t="s">
         <v>298</v>
       </c>
@@ -13207,7 +13229,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="15" customHeight="1">
+    <row r="193" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="15" t="s">
         <v>412</v>
       </c>
@@ -13258,7 +13280,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="15" customHeight="1">
+    <row r="194" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="15" t="s">
         <v>299</v>
       </c>
@@ -13308,7 +13330,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="15" customHeight="1">
+    <row r="195" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="15" t="s">
         <v>300</v>
       </c>
@@ -13358,7 +13380,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="15" t="s">
         <v>301</v>
       </c>
@@ -13409,7 +13431,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A197" s="15" t="s">
         <v>304</v>
       </c>
@@ -13460,7 +13482,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A198" s="15" t="s">
         <v>306</v>
       </c>
@@ -13510,7 +13532,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A199" s="15" t="s">
         <v>309</v>
       </c>
@@ -13561,7 +13583,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A200" s="15" t="s">
         <v>310</v>
       </c>
@@ -13612,7 +13634,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="29.25" customHeight="1">
+    <row r="201" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="15" t="s">
         <v>311</v>
       </c>
@@ -13663,7 +13685,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="42">
+    <row r="202" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A202" s="15" t="s">
         <v>407</v>
       </c>
@@ -13714,7 +13736,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="15" t="s">
         <v>408</v>
       </c>
@@ -13764,7 +13786,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A204" s="15" t="s">
         <v>315</v>
       </c>
@@ -13815,7 +13837,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="42">
+    <row r="205" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A205" s="15" t="s">
         <v>406</v>
       </c>
@@ -13866,7 +13888,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="28">
+    <row r="206" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A206" s="15" t="s">
         <v>317</v>
       </c>
@@ -13917,7 +13939,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A207" s="15" t="s">
         <v>319</v>
       </c>
@@ -13968,7 +13990,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A208" s="15" t="s">
         <v>320</v>
       </c>
@@ -14018,7 +14040,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A209" s="15" t="s">
         <v>321</v>
       </c>
@@ -14069,7 +14091,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A210" s="15" t="s">
         <v>322</v>
       </c>
@@ -14119,7 +14141,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A211" s="15" t="s">
         <v>323</v>
       </c>
@@ -14170,7 +14192,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A212" s="15" t="s">
         <v>324</v>
       </c>
@@ -14221,7 +14243,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A213" s="15" t="s">
         <v>325</v>
       </c>
@@ -14272,7 +14294,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A214" s="15" t="s">
         <v>326</v>
       </c>
@@ -14322,7 +14344,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A215" s="15" t="s">
         <v>328</v>
       </c>
@@ -14372,7 +14394,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A216" s="15" t="s">
         <v>329</v>
       </c>
@@ -14422,7 +14444,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A217" s="15" t="s">
         <v>331</v>
       </c>
@@ -14473,7 +14495,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A218" s="15" t="s">
         <v>332</v>
       </c>
@@ -14524,7 +14546,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="28">
+    <row r="219" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="15" t="s">
         <v>364</v>
       </c>
@@ -14574,7 +14596,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A220" s="15" t="s">
         <v>333</v>
       </c>
@@ -14624,7 +14646,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A221" s="15" t="s">
         <v>336</v>
       </c>
@@ -14674,7 +14696,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="28">
+    <row r="222" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="15" t="s">
         <v>337</v>
       </c>
@@ -14725,7 +14747,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A223" s="15" t="s">
         <v>341</v>
       </c>
@@ -14776,7 +14798,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A224" s="15" t="s">
         <v>342</v>
       </c>
@@ -14827,7 +14849,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="15.75" customHeight="1">
+    <row r="225" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="15" t="s">
         <v>343</v>
       </c>
@@ -14878,7 +14900,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="226" spans="1:19">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A226" s="15" t="s">
         <v>344</v>
       </c>
@@ -14929,7 +14951,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="227" spans="1:19">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A227" s="15" t="s">
         <v>345</v>
       </c>
@@ -14979,7 +15001,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="228" spans="1:19">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A228" s="15" t="s">
         <v>346</v>
       </c>
@@ -15030,7 +15052,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="229" spans="1:19">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A229" s="15" t="s">
         <v>347</v>
       </c>
@@ -15081,7 +15103,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="230" spans="1:19">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A230" s="15" t="s">
         <v>348</v>
       </c>
@@ -15132,7 +15154,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="231" spans="1:19">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A231" s="15" t="s">
         <v>349</v>
       </c>
@@ -15183,7 +15205,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="232" spans="1:19">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A232" s="15" t="s">
         <v>350</v>
       </c>
@@ -15234,7 +15256,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="233" spans="1:19">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A233" s="15" t="s">
         <v>405</v>
       </c>
@@ -15284,7 +15306,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="234" spans="1:19">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A234" s="15" t="s">
         <v>416</v>
       </c>
@@ -15334,7 +15356,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="235" spans="1:19">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A235" s="15" t="s">
         <v>418</v>
       </c>
@@ -15384,7 +15406,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="236" spans="1:19">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A236" s="15" t="s">
         <v>419</v>
       </c>
@@ -15434,7 +15456,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="237" spans="1:19">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A237" s="15" t="s">
         <v>420</v>
       </c>
@@ -15484,7 +15506,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="238" spans="1:19">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A238" s="15" t="s">
         <v>421</v>
       </c>
@@ -15534,7 +15556,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="25">
+    <row r="239" spans="1:19" ht="26" x14ac:dyDescent="0.35">
       <c r="A239" s="17" t="s">
         <v>396</v>
       </c>
@@ -15587,7 +15609,7 @@
       <c r="R239" s="12"/>
       <c r="S239" s="12"/>
     </row>
-    <row r="240" spans="1:19" ht="25">
+    <row r="240" spans="1:19" ht="26" x14ac:dyDescent="0.35">
       <c r="A240" s="17" t="s">
         <v>400</v>
       </c>
@@ -15640,7 +15662,7 @@
       <c r="R240" s="12"/>
       <c r="S240" s="12"/>
     </row>
-    <row r="241" spans="1:19" ht="25">
+    <row r="241" spans="1:19" ht="26" x14ac:dyDescent="0.35">
       <c r="A241" s="17" t="s">
         <v>389</v>
       </c>
@@ -15693,7 +15715,7 @@
       <c r="R241" s="12"/>
       <c r="S241" s="12"/>
     </row>
-    <row r="242" spans="1:19" ht="25">
+    <row r="242" spans="1:19" ht="26" x14ac:dyDescent="0.35">
       <c r="A242" s="17" t="s">
         <v>392</v>
       </c>
@@ -15746,7 +15768,7 @@
       <c r="R242" s="12"/>
       <c r="S242" s="12"/>
     </row>
-    <row r="243" spans="1:19" ht="25">
+    <row r="243" spans="1:19" ht="26" x14ac:dyDescent="0.35">
       <c r="A243" s="17" t="s">
         <v>394</v>
       </c>
@@ -15800,7 +15822,6 @@
       <c r="S243" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S243"/>
   <sortState ref="A2:S243">
     <sortCondition ref="A2:A243"/>
   </sortState>

</xml_diff>